<commit_message>
Eliminados los 0s en el formato de bachillerato
</commit_message>
<xml_diff>
--- a/public/formato_bac.xlsx
+++ b/public/formato_bac.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web\uc\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ECD0524-C9D3-476F-BDC7-27105EA626FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB7D0BEE-D623-4D64-8C57-D79D1A3D362A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7F88D77E-4E3E-48C4-9DAA-2646452AF6C7}"/>
   </bookViews>
@@ -733,29 +733,51 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -797,28 +819,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1401,20 +1401,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1423,9 +1423,9 @@
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
       <c r="G2" s="32"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -1435,20 +1435,20 @@
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
       <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -1458,110 +1458,110 @@
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
       <c r="K5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="52" t="s">
+      <c r="L5" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="52"/>
+      <c r="M5" s="53"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="8"/>
       <c r="K6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="9"/>
       <c r="K7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
     </row>
     <row r="8" spans="1:13" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:13" s="11" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="61" t="s">
+      <c r="E9" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="50"/>
-      <c r="H9" s="63" t="s">
+      <c r="G9" s="58"/>
+      <c r="H9" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="63" t="s">
+      <c r="I9" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="65" t="s">
+      <c r="J9" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="66"/>
-      <c r="L9" s="65" t="s">
+      <c r="K9" s="72"/>
+      <c r="L9" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="66"/>
+      <c r="M9" s="72"/>
     </row>
     <row r="10" spans="1:13" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="54"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="62"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="68"/>
       <c r="F10" s="35" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
       <c r="J10" s="12" t="s">
         <v>18</v>
       </c>
@@ -1582,21 +1582,11 @@
       <c r="B11" s="15"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
-      <c r="E11" s="72">
-        <v>0</v>
-      </c>
-      <c r="F11" s="72">
-        <v>0</v>
-      </c>
-      <c r="G11" s="72">
-        <v>0</v>
-      </c>
-      <c r="H11" s="72">
-        <v>0</v>
-      </c>
-      <c r="I11" s="72">
-        <v>0</v>
-      </c>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
       <c r="J11" s="37"/>
       <c r="K11" s="38" t="s">
         <v>20</v>
@@ -1613,21 +1603,11 @@
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
-      <c r="E12" s="72">
-        <v>0</v>
-      </c>
-      <c r="F12" s="72">
-        <v>0</v>
-      </c>
-      <c r="G12" s="72">
-        <v>0</v>
-      </c>
-      <c r="H12" s="72">
-        <v>0</v>
-      </c>
-      <c r="I12" s="72">
-        <v>0</v>
-      </c>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
       <c r="J12" s="39"/>
       <c r="K12" s="38" t="s">
         <v>20</v>
@@ -1644,21 +1624,11 @@
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
-      <c r="E13" s="72">
-        <v>0</v>
-      </c>
-      <c r="F13" s="72">
-        <v>0</v>
-      </c>
-      <c r="G13" s="72">
-        <v>0</v>
-      </c>
-      <c r="H13" s="72">
-        <v>0</v>
-      </c>
-      <c r="I13" s="72">
-        <v>0</v>
-      </c>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
       <c r="J13" s="39"/>
       <c r="K13" s="38" t="s">
         <v>20</v>
@@ -1675,21 +1645,11 @@
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
-      <c r="E14" s="72">
-        <v>0</v>
-      </c>
-      <c r="F14" s="72">
-        <v>0</v>
-      </c>
-      <c r="G14" s="72">
-        <v>0</v>
-      </c>
-      <c r="H14" s="72">
-        <v>0</v>
-      </c>
-      <c r="I14" s="72">
-        <v>0</v>
-      </c>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
       <c r="J14" s="39"/>
       <c r="K14" s="38" t="s">
         <v>20</v>
@@ -1706,21 +1666,11 @@
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
-      <c r="E15" s="72">
-        <v>0</v>
-      </c>
-      <c r="F15" s="72">
-        <v>0</v>
-      </c>
-      <c r="G15" s="72">
-        <v>0</v>
-      </c>
-      <c r="H15" s="72">
-        <v>0</v>
-      </c>
-      <c r="I15" s="72">
-        <v>0</v>
-      </c>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
       <c r="J15" s="39"/>
       <c r="K15" s="38" t="s">
         <v>20</v>
@@ -1737,21 +1687,11 @@
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
-      <c r="E16" s="72">
-        <v>0</v>
-      </c>
-      <c r="F16" s="72">
-        <v>0</v>
-      </c>
-      <c r="G16" s="72">
-        <v>0</v>
-      </c>
-      <c r="H16" s="72">
-        <v>0</v>
-      </c>
-      <c r="I16" s="72">
-        <v>0</v>
-      </c>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
       <c r="J16" s="39"/>
       <c r="K16" s="38" t="s">
         <v>20</v>
@@ -1768,21 +1708,11 @@
       <c r="B17" s="18"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
-      <c r="E17" s="72">
-        <v>0</v>
-      </c>
-      <c r="F17" s="72">
-        <v>0</v>
-      </c>
-      <c r="G17" s="72">
-        <v>0</v>
-      </c>
-      <c r="H17" s="72">
-        <v>0</v>
-      </c>
-      <c r="I17" s="72">
-        <v>0</v>
-      </c>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="39"/>
       <c r="K17" s="38" t="s">
         <v>20</v>
@@ -1799,21 +1729,11 @@
       <c r="B18" s="18"/>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
-      <c r="E18" s="72">
-        <v>0</v>
-      </c>
-      <c r="F18" s="72">
-        <v>0</v>
-      </c>
-      <c r="G18" s="72">
-        <v>0</v>
-      </c>
-      <c r="H18" s="72">
-        <v>0</v>
-      </c>
-      <c r="I18" s="72">
-        <v>0</v>
-      </c>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
       <c r="J18" s="39"/>
       <c r="K18" s="38" t="s">
         <v>20</v>
@@ -1830,21 +1750,11 @@
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
-      <c r="E19" s="72">
-        <v>0</v>
-      </c>
-      <c r="F19" s="72">
-        <v>0</v>
-      </c>
-      <c r="G19" s="72">
-        <v>0</v>
-      </c>
-      <c r="H19" s="72">
-        <v>0</v>
-      </c>
-      <c r="I19" s="72">
-        <v>0</v>
-      </c>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
       <c r="J19" s="39"/>
       <c r="K19" s="38" t="s">
         <v>20</v>
@@ -1861,21 +1771,11 @@
       <c r="B20" s="18"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
-      <c r="E20" s="72">
-        <v>0</v>
-      </c>
-      <c r="F20" s="72">
-        <v>0</v>
-      </c>
-      <c r="G20" s="72">
-        <v>0</v>
-      </c>
-      <c r="H20" s="72">
-        <v>0</v>
-      </c>
-      <c r="I20" s="72">
-        <v>0</v>
-      </c>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
       <c r="J20" s="39"/>
       <c r="K20" s="38" t="s">
         <v>20</v>
@@ -1892,21 +1792,11 @@
       <c r="B21" s="18"/>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
-      <c r="E21" s="72">
-        <v>0</v>
-      </c>
-      <c r="F21" s="72">
-        <v>0</v>
-      </c>
-      <c r="G21" s="72">
-        <v>0</v>
-      </c>
-      <c r="H21" s="72">
-        <v>0</v>
-      </c>
-      <c r="I21" s="72">
-        <v>0</v>
-      </c>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
       <c r="J21" s="39"/>
       <c r="K21" s="38" t="s">
         <v>20</v>
@@ -1923,21 +1813,11 @@
       <c r="B22" s="18"/>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
-      <c r="E22" s="72">
-        <v>0</v>
-      </c>
-      <c r="F22" s="72">
-        <v>0</v>
-      </c>
-      <c r="G22" s="72">
-        <v>0</v>
-      </c>
-      <c r="H22" s="72">
-        <v>0</v>
-      </c>
-      <c r="I22" s="72">
-        <v>0</v>
-      </c>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
       <c r="J22" s="39"/>
       <c r="K22" s="38" t="s">
         <v>20</v>
@@ -1954,21 +1834,11 @@
       <c r="B23" s="18"/>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
-      <c r="E23" s="72">
-        <v>0</v>
-      </c>
-      <c r="F23" s="72">
-        <v>0</v>
-      </c>
-      <c r="G23" s="72">
-        <v>0</v>
-      </c>
-      <c r="H23" s="72">
-        <v>0</v>
-      </c>
-      <c r="I23" s="72">
-        <v>0</v>
-      </c>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
       <c r="J23" s="39"/>
       <c r="K23" s="38" t="s">
         <v>20</v>
@@ -1985,21 +1855,11 @@
       <c r="B24" s="20"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
-      <c r="E24" s="72">
-        <v>0</v>
-      </c>
-      <c r="F24" s="72">
-        <v>0</v>
-      </c>
-      <c r="G24" s="72">
-        <v>0</v>
-      </c>
-      <c r="H24" s="72">
-        <v>0</v>
-      </c>
-      <c r="I24" s="72">
-        <v>0</v>
-      </c>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
       <c r="J24" s="40"/>
       <c r="K24" s="38" t="s">
         <v>20</v>
@@ -2016,21 +1876,11 @@
       <c r="B25" s="20"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
-      <c r="E25" s="72">
-        <v>0</v>
-      </c>
-      <c r="F25" s="72">
-        <v>0</v>
-      </c>
-      <c r="G25" s="72">
-        <v>0</v>
-      </c>
-      <c r="H25" s="72">
-        <v>0</v>
-      </c>
-      <c r="I25" s="72">
-        <v>0</v>
-      </c>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
       <c r="J25" s="40"/>
       <c r="K25" s="38" t="s">
         <v>20</v>
@@ -2047,21 +1897,11 @@
       <c r="B26" s="20"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
-      <c r="E26" s="72">
-        <v>0</v>
-      </c>
-      <c r="F26" s="72">
-        <v>0</v>
-      </c>
-      <c r="G26" s="72">
-        <v>0</v>
-      </c>
-      <c r="H26" s="72">
-        <v>0</v>
-      </c>
-      <c r="I26" s="72">
-        <v>0</v>
-      </c>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
       <c r="J26" s="41"/>
       <c r="K26" s="38" t="s">
         <v>20</v>
@@ -2078,21 +1918,11 @@
       <c r="B27" s="20"/>
       <c r="C27" s="21"/>
       <c r="D27" s="21"/>
-      <c r="E27" s="72">
-        <v>0</v>
-      </c>
-      <c r="F27" s="72">
-        <v>0</v>
-      </c>
-      <c r="G27" s="72">
-        <v>0</v>
-      </c>
-      <c r="H27" s="72">
-        <v>0</v>
-      </c>
-      <c r="I27" s="72">
-        <v>0</v>
-      </c>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
       <c r="J27" s="40"/>
       <c r="K27" s="38" t="s">
         <v>20</v>
@@ -2109,21 +1939,11 @@
       <c r="B28" s="20"/>
       <c r="C28" s="21"/>
       <c r="D28" s="21"/>
-      <c r="E28" s="72">
-        <v>0</v>
-      </c>
-      <c r="F28" s="72">
-        <v>0</v>
-      </c>
-      <c r="G28" s="72">
-        <v>0</v>
-      </c>
-      <c r="H28" s="72">
-        <v>0</v>
-      </c>
-      <c r="I28" s="72">
-        <v>0</v>
-      </c>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
       <c r="J28" s="41"/>
       <c r="K28" s="38" t="s">
         <v>20</v>
@@ -2140,21 +1960,11 @@
       <c r="B29" s="20"/>
       <c r="C29" s="21"/>
       <c r="D29" s="21"/>
-      <c r="E29" s="72">
-        <v>0</v>
-      </c>
-      <c r="F29" s="72">
-        <v>0</v>
-      </c>
-      <c r="G29" s="72">
-        <v>0</v>
-      </c>
-      <c r="H29" s="72">
-        <v>0</v>
-      </c>
-      <c r="I29" s="72">
-        <v>0</v>
-      </c>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
       <c r="J29" s="41"/>
       <c r="K29" s="38" t="s">
         <v>20</v>
@@ -2171,21 +1981,11 @@
       <c r="B30" s="20"/>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
-      <c r="E30" s="72">
-        <v>0</v>
-      </c>
-      <c r="F30" s="72">
-        <v>0</v>
-      </c>
-      <c r="G30" s="72">
-        <v>0</v>
-      </c>
-      <c r="H30" s="72">
-        <v>0</v>
-      </c>
-      <c r="I30" s="72">
-        <v>0</v>
-      </c>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
       <c r="J30" s="41"/>
       <c r="K30" s="38" t="s">
         <v>20</v>
@@ -2202,21 +2002,11 @@
       <c r="B31" s="20"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
-      <c r="E31" s="72">
-        <v>0</v>
-      </c>
-      <c r="F31" s="72">
-        <v>0</v>
-      </c>
-      <c r="G31" s="72">
-        <v>0</v>
-      </c>
-      <c r="H31" s="72">
-        <v>0</v>
-      </c>
-      <c r="I31" s="72">
-        <v>0</v>
-      </c>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
       <c r="J31" s="41"/>
       <c r="K31" s="38" t="s">
         <v>20</v>
@@ -2233,21 +2023,11 @@
       <c r="B32" s="20"/>
       <c r="C32" s="21"/>
       <c r="D32" s="21"/>
-      <c r="E32" s="72">
-        <v>0</v>
-      </c>
-      <c r="F32" s="72">
-        <v>0</v>
-      </c>
-      <c r="G32" s="72">
-        <v>0</v>
-      </c>
-      <c r="H32" s="72">
-        <v>0</v>
-      </c>
-      <c r="I32" s="72">
-        <v>0</v>
-      </c>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
       <c r="J32" s="40"/>
       <c r="K32" s="38" t="s">
         <v>20</v>
@@ -2264,21 +2044,11 @@
       <c r="B33" s="20"/>
       <c r="C33" s="21"/>
       <c r="D33" s="21"/>
-      <c r="E33" s="72">
-        <v>0</v>
-      </c>
-      <c r="F33" s="72">
-        <v>0</v>
-      </c>
-      <c r="G33" s="72">
-        <v>0</v>
-      </c>
-      <c r="H33" s="72">
-        <v>0</v>
-      </c>
-      <c r="I33" s="72">
-        <v>0</v>
-      </c>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
       <c r="J33" s="40"/>
       <c r="K33" s="38" t="s">
         <v>20</v>
@@ -2295,21 +2065,11 @@
       <c r="B34" s="20"/>
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
-      <c r="E34" s="72">
-        <v>0</v>
-      </c>
-      <c r="F34" s="72">
-        <v>0</v>
-      </c>
-      <c r="G34" s="72">
-        <v>0</v>
-      </c>
-      <c r="H34" s="72">
-        <v>0</v>
-      </c>
-      <c r="I34" s="72">
-        <v>0</v>
-      </c>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
       <c r="J34" s="41"/>
       <c r="K34" s="38" t="s">
         <v>20</v>
@@ -2326,21 +2086,11 @@
       <c r="B35" s="20"/>
       <c r="C35" s="21"/>
       <c r="D35" s="21"/>
-      <c r="E35" s="72">
-        <v>0</v>
-      </c>
-      <c r="F35" s="72">
-        <v>0</v>
-      </c>
-      <c r="G35" s="72">
-        <v>0</v>
-      </c>
-      <c r="H35" s="72">
-        <v>0</v>
-      </c>
-      <c r="I35" s="72">
-        <v>0</v>
-      </c>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
       <c r="J35" s="40"/>
       <c r="K35" s="38" t="s">
         <v>20</v>
@@ -2357,21 +2107,11 @@
       <c r="B36" s="20"/>
       <c r="C36" s="21"/>
       <c r="D36" s="21"/>
-      <c r="E36" s="72">
-        <v>0</v>
-      </c>
-      <c r="F36" s="72">
-        <v>0</v>
-      </c>
-      <c r="G36" s="72">
-        <v>0</v>
-      </c>
-      <c r="H36" s="72">
-        <v>0</v>
-      </c>
-      <c r="I36" s="72">
-        <v>0</v>
-      </c>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
       <c r="J36" s="41"/>
       <c r="K36" s="38" t="s">
         <v>20</v>
@@ -2388,21 +2128,11 @@
       <c r="B37" s="20"/>
       <c r="C37" s="21"/>
       <c r="D37" s="21"/>
-      <c r="E37" s="72">
-        <v>0</v>
-      </c>
-      <c r="F37" s="72">
-        <v>0</v>
-      </c>
-      <c r="G37" s="72">
-        <v>0</v>
-      </c>
-      <c r="H37" s="72">
-        <v>0</v>
-      </c>
-      <c r="I37" s="72">
-        <v>0</v>
-      </c>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
       <c r="J37" s="41"/>
       <c r="K37" s="38" t="s">
         <v>20</v>
@@ -2419,21 +2149,11 @@
       <c r="B38" s="20"/>
       <c r="C38" s="21"/>
       <c r="D38" s="21"/>
-      <c r="E38" s="72">
-        <v>0</v>
-      </c>
-      <c r="F38" s="72">
-        <v>0</v>
-      </c>
-      <c r="G38" s="72">
-        <v>0</v>
-      </c>
-      <c r="H38" s="72">
-        <v>0</v>
-      </c>
-      <c r="I38" s="72">
-        <v>0</v>
-      </c>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
       <c r="J38" s="41"/>
       <c r="K38" s="38" t="s">
         <v>20</v>
@@ -2450,21 +2170,11 @@
       <c r="B39" s="20"/>
       <c r="C39" s="21"/>
       <c r="D39" s="21"/>
-      <c r="E39" s="72">
-        <v>0</v>
-      </c>
-      <c r="F39" s="72">
-        <v>0</v>
-      </c>
-      <c r="G39" s="72">
-        <v>0</v>
-      </c>
-      <c r="H39" s="72">
-        <v>0</v>
-      </c>
-      <c r="I39" s="72">
-        <v>0</v>
-      </c>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
       <c r="J39" s="40"/>
       <c r="K39" s="38" t="s">
         <v>20</v>
@@ -2481,21 +2191,11 @@
       <c r="B40" s="20"/>
       <c r="C40" s="21"/>
       <c r="D40" s="21"/>
-      <c r="E40" s="72">
-        <v>0</v>
-      </c>
-      <c r="F40" s="72">
-        <v>0</v>
-      </c>
-      <c r="G40" s="72">
-        <v>0</v>
-      </c>
-      <c r="H40" s="72">
-        <v>0</v>
-      </c>
-      <c r="I40" s="72">
-        <v>0</v>
-      </c>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
       <c r="J40" s="40"/>
       <c r="K40" s="38" t="s">
         <v>20</v>
@@ -2512,21 +2212,11 @@
       <c r="B41" s="20"/>
       <c r="C41" s="21"/>
       <c r="D41" s="21"/>
-      <c r="E41" s="72">
-        <v>0</v>
-      </c>
-      <c r="F41" s="72">
-        <v>0</v>
-      </c>
-      <c r="G41" s="72">
-        <v>0</v>
-      </c>
-      <c r="H41" s="72">
-        <v>0</v>
-      </c>
-      <c r="I41" s="72">
-        <v>0</v>
-      </c>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="46"/>
       <c r="J41" s="40"/>
       <c r="K41" s="38" t="s">
         <v>20</v>
@@ -2543,21 +2233,11 @@
       <c r="B42" s="20"/>
       <c r="C42" s="21"/>
       <c r="D42" s="21"/>
-      <c r="E42" s="72">
-        <v>0</v>
-      </c>
-      <c r="F42" s="72">
-        <v>0</v>
-      </c>
-      <c r="G42" s="72">
-        <v>0</v>
-      </c>
-      <c r="H42" s="72">
-        <v>0</v>
-      </c>
-      <c r="I42" s="72">
-        <v>0</v>
-      </c>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
       <c r="J42" s="41"/>
       <c r="K42" s="38" t="s">
         <v>20</v>
@@ -2574,21 +2254,11 @@
       <c r="B43" s="20"/>
       <c r="C43" s="21"/>
       <c r="D43" s="21"/>
-      <c r="E43" s="72">
-        <v>0</v>
-      </c>
-      <c r="F43" s="72">
-        <v>0</v>
-      </c>
-      <c r="G43" s="72">
-        <v>0</v>
-      </c>
-      <c r="H43" s="72">
-        <v>0</v>
-      </c>
-      <c r="I43" s="72">
-        <v>0</v>
-      </c>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="46"/>
       <c r="J43" s="40"/>
       <c r="K43" s="38" t="s">
         <v>20</v>
@@ -2605,21 +2275,11 @@
       <c r="B44" s="20"/>
       <c r="C44" s="21"/>
       <c r="D44" s="21"/>
-      <c r="E44" s="72">
-        <v>0</v>
-      </c>
-      <c r="F44" s="72">
-        <v>0</v>
-      </c>
-      <c r="G44" s="72">
-        <v>0</v>
-      </c>
-      <c r="H44" s="72">
-        <v>0</v>
-      </c>
-      <c r="I44" s="72">
-        <v>0</v>
-      </c>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="46"/>
       <c r="J44" s="41"/>
       <c r="K44" s="38" t="s">
         <v>20</v>
@@ -2636,21 +2296,11 @@
       <c r="B45" s="20"/>
       <c r="C45" s="21"/>
       <c r="D45" s="21"/>
-      <c r="E45" s="72">
-        <v>0</v>
-      </c>
-      <c r="F45" s="72">
-        <v>0</v>
-      </c>
-      <c r="G45" s="72">
-        <v>0</v>
-      </c>
-      <c r="H45" s="72">
-        <v>0</v>
-      </c>
-      <c r="I45" s="72">
-        <v>0</v>
-      </c>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="46"/>
       <c r="J45" s="40"/>
       <c r="K45" s="38" t="s">
         <v>20</v>
@@ -2667,21 +2317,11 @@
       <c r="B46" s="22"/>
       <c r="C46" s="21"/>
       <c r="D46" s="21"/>
-      <c r="E46" s="72">
-        <v>0</v>
-      </c>
-      <c r="F46" s="72">
-        <v>0</v>
-      </c>
-      <c r="G46" s="72">
-        <v>0</v>
-      </c>
-      <c r="H46" s="72">
-        <v>0</v>
-      </c>
-      <c r="I46" s="72">
-        <v>0</v>
-      </c>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="46"/>
       <c r="J46" s="41"/>
       <c r="K46" s="38" t="s">
         <v>20</v>
@@ -2698,21 +2338,11 @@
       <c r="B47" s="22"/>
       <c r="C47" s="21"/>
       <c r="D47" s="21"/>
-      <c r="E47" s="72">
-        <v>0</v>
-      </c>
-      <c r="F47" s="72">
-        <v>0</v>
-      </c>
-      <c r="G47" s="72">
-        <v>0</v>
-      </c>
-      <c r="H47" s="72">
-        <v>0</v>
-      </c>
-      <c r="I47" s="72">
-        <v>0</v>
-      </c>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
       <c r="J47" s="41"/>
       <c r="K47" s="38" t="s">
         <v>20</v>
@@ -2729,21 +2359,11 @@
       <c r="B48" s="22"/>
       <c r="C48" s="21"/>
       <c r="D48" s="21"/>
-      <c r="E48" s="72">
-        <v>0</v>
-      </c>
-      <c r="F48" s="72">
-        <v>0</v>
-      </c>
-      <c r="G48" s="72">
-        <v>0</v>
-      </c>
-      <c r="H48" s="72">
-        <v>0</v>
-      </c>
-      <c r="I48" s="72">
-        <v>0</v>
-      </c>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="46"/>
       <c r="J48" s="41"/>
       <c r="K48" s="38" t="s">
         <v>20</v>
@@ -2760,21 +2380,11 @@
       <c r="B49" s="22"/>
       <c r="C49" s="21"/>
       <c r="D49" s="21"/>
-      <c r="E49" s="72">
-        <v>0</v>
-      </c>
-      <c r="F49" s="72">
-        <v>0</v>
-      </c>
-      <c r="G49" s="72">
-        <v>0</v>
-      </c>
-      <c r="H49" s="72">
-        <v>0</v>
-      </c>
-      <c r="I49" s="72">
-        <v>0</v>
-      </c>
+      <c r="E49" s="46"/>
+      <c r="F49" s="46"/>
+      <c r="G49" s="46"/>
+      <c r="H49" s="46"/>
+      <c r="I49" s="46"/>
       <c r="J49" s="41"/>
       <c r="K49" s="38" t="s">
         <v>20</v>
@@ -2791,21 +2401,11 @@
       <c r="B50" s="22"/>
       <c r="C50" s="21"/>
       <c r="D50" s="21"/>
-      <c r="E50" s="72">
-        <v>0</v>
-      </c>
-      <c r="F50" s="72">
-        <v>0</v>
-      </c>
-      <c r="G50" s="72">
-        <v>0</v>
-      </c>
-      <c r="H50" s="72">
-        <v>0</v>
-      </c>
-      <c r="I50" s="72">
-        <v>0</v>
-      </c>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
       <c r="J50" s="41"/>
       <c r="K50" s="38" t="s">
         <v>20</v>
@@ -2822,21 +2422,11 @@
       <c r="B51" s="22"/>
       <c r="C51" s="21"/>
       <c r="D51" s="21"/>
-      <c r="E51" s="72">
-        <v>0</v>
-      </c>
-      <c r="F51" s="72">
-        <v>0</v>
-      </c>
-      <c r="G51" s="72">
-        <v>0</v>
-      </c>
-      <c r="H51" s="72">
-        <v>0</v>
-      </c>
-      <c r="I51" s="72">
-        <v>0</v>
-      </c>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="46"/>
       <c r="J51" s="41"/>
       <c r="K51" s="38" t="s">
         <v>20</v>
@@ -2853,21 +2443,11 @@
       <c r="B52" s="22"/>
       <c r="C52" s="21"/>
       <c r="D52" s="21"/>
-      <c r="E52" s="72">
-        <v>0</v>
-      </c>
-      <c r="F52" s="72">
-        <v>0</v>
-      </c>
-      <c r="G52" s="72">
-        <v>0</v>
-      </c>
-      <c r="H52" s="72">
-        <v>0</v>
-      </c>
-      <c r="I52" s="72">
-        <v>0</v>
-      </c>
+      <c r="E52" s="46"/>
+      <c r="F52" s="46"/>
+      <c r="G52" s="46"/>
+      <c r="H52" s="46"/>
+      <c r="I52" s="46"/>
       <c r="J52" s="41"/>
       <c r="K52" s="38" t="s">
         <v>20</v>
@@ -2884,21 +2464,11 @@
       <c r="B53" s="22"/>
       <c r="C53" s="21"/>
       <c r="D53" s="21"/>
-      <c r="E53" s="72">
-        <v>0</v>
-      </c>
-      <c r="F53" s="72">
-        <v>0</v>
-      </c>
-      <c r="G53" s="72">
-        <v>0</v>
-      </c>
-      <c r="H53" s="72">
-        <v>0</v>
-      </c>
-      <c r="I53" s="72">
-        <v>0</v>
-      </c>
+      <c r="E53" s="46"/>
+      <c r="F53" s="46"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="46"/>
       <c r="J53" s="41"/>
       <c r="K53" s="38" t="s">
         <v>20</v>
@@ -2915,21 +2485,11 @@
       <c r="B54" s="22"/>
       <c r="C54" s="21"/>
       <c r="D54" s="21"/>
-      <c r="E54" s="72">
-        <v>0</v>
-      </c>
-      <c r="F54" s="72">
-        <v>0</v>
-      </c>
-      <c r="G54" s="72">
-        <v>0</v>
-      </c>
-      <c r="H54" s="72">
-        <v>0</v>
-      </c>
-      <c r="I54" s="72">
-        <v>0</v>
-      </c>
+      <c r="E54" s="46"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
       <c r="J54" s="41"/>
       <c r="K54" s="38" t="s">
         <v>20</v>
@@ -2946,21 +2506,11 @@
       <c r="B55" s="22"/>
       <c r="C55" s="21"/>
       <c r="D55" s="21"/>
-      <c r="E55" s="72">
-        <v>0</v>
-      </c>
-      <c r="F55" s="72">
-        <v>0</v>
-      </c>
-      <c r="G55" s="72">
-        <v>0</v>
-      </c>
-      <c r="H55" s="72">
-        <v>0</v>
-      </c>
-      <c r="I55" s="72">
-        <v>0</v>
-      </c>
+      <c r="E55" s="46"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="46"/>
+      <c r="H55" s="46"/>
+      <c r="I55" s="46"/>
       <c r="J55" s="41"/>
       <c r="K55" s="38" t="s">
         <v>20</v>
@@ -2977,21 +2527,11 @@
       <c r="B56" s="22"/>
       <c r="C56" s="21"/>
       <c r="D56" s="21"/>
-      <c r="E56" s="72">
-        <v>0</v>
-      </c>
-      <c r="F56" s="72">
-        <v>0</v>
-      </c>
-      <c r="G56" s="72">
-        <v>0</v>
-      </c>
-      <c r="H56" s="72">
-        <v>0</v>
-      </c>
-      <c r="I56" s="72">
-        <v>0</v>
-      </c>
+      <c r="E56" s="46"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="46"/>
+      <c r="H56" s="46"/>
+      <c r="I56" s="46"/>
       <c r="J56" s="41"/>
       <c r="K56" s="38" t="s">
         <v>20</v>
@@ -3008,21 +2548,11 @@
       <c r="B57" s="22"/>
       <c r="C57" s="21"/>
       <c r="D57" s="21"/>
-      <c r="E57" s="72">
-        <v>0</v>
-      </c>
-      <c r="F57" s="72">
-        <v>0</v>
-      </c>
-      <c r="G57" s="72">
-        <v>0</v>
-      </c>
-      <c r="H57" s="72">
-        <v>0</v>
-      </c>
-      <c r="I57" s="72">
-        <v>0</v>
-      </c>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="46"/>
+      <c r="I57" s="46"/>
       <c r="J57" s="41"/>
       <c r="K57" s="38" t="s">
         <v>20</v>
@@ -3039,21 +2569,11 @@
       <c r="B58" s="22"/>
       <c r="C58" s="21"/>
       <c r="D58" s="21"/>
-      <c r="E58" s="72">
-        <v>0</v>
-      </c>
-      <c r="F58" s="72">
-        <v>0</v>
-      </c>
-      <c r="G58" s="72">
-        <v>0</v>
-      </c>
-      <c r="H58" s="72">
-        <v>0</v>
-      </c>
-      <c r="I58" s="72">
-        <v>0</v>
-      </c>
+      <c r="E58" s="46"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="46"/>
       <c r="J58" s="41"/>
       <c r="K58" s="38" t="s">
         <v>20</v>
@@ -3070,21 +2590,11 @@
       <c r="B59" s="22"/>
       <c r="C59" s="21"/>
       <c r="D59" s="21"/>
-      <c r="E59" s="72">
-        <v>0</v>
-      </c>
-      <c r="F59" s="72">
-        <v>0</v>
-      </c>
-      <c r="G59" s="72">
-        <v>0</v>
-      </c>
-      <c r="H59" s="72">
-        <v>0</v>
-      </c>
-      <c r="I59" s="72">
-        <v>0</v>
-      </c>
+      <c r="E59" s="46"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="46"/>
+      <c r="H59" s="46"/>
+      <c r="I59" s="46"/>
       <c r="J59" s="41"/>
       <c r="K59" s="38" t="s">
         <v>20</v>
@@ -3101,21 +2611,11 @@
       <c r="B60" s="22"/>
       <c r="C60" s="21"/>
       <c r="D60" s="21"/>
-      <c r="E60" s="72">
-        <v>0</v>
-      </c>
-      <c r="F60" s="72">
-        <v>0</v>
-      </c>
-      <c r="G60" s="72">
-        <v>0</v>
-      </c>
-      <c r="H60" s="72">
-        <v>0</v>
-      </c>
-      <c r="I60" s="72">
-        <v>0</v>
-      </c>
+      <c r="E60" s="46"/>
+      <c r="F60" s="46"/>
+      <c r="G60" s="46"/>
+      <c r="H60" s="46"/>
+      <c r="I60" s="46"/>
       <c r="J60" s="41"/>
       <c r="K60" s="38" t="s">
         <v>20</v>
@@ -3132,21 +2632,11 @@
       <c r="B61" s="22"/>
       <c r="C61" s="21"/>
       <c r="D61" s="21"/>
-      <c r="E61" s="72">
-        <v>0</v>
-      </c>
-      <c r="F61" s="72">
-        <v>0</v>
-      </c>
-      <c r="G61" s="72">
-        <v>0</v>
-      </c>
-      <c r="H61" s="72">
-        <v>0</v>
-      </c>
-      <c r="I61" s="72">
-        <v>0</v>
-      </c>
+      <c r="E61" s="46"/>
+      <c r="F61" s="46"/>
+      <c r="G61" s="46"/>
+      <c r="H61" s="46"/>
+      <c r="I61" s="46"/>
       <c r="J61" s="41"/>
       <c r="K61" s="38" t="s">
         <v>20</v>
@@ -3163,21 +2653,11 @@
       <c r="B62" s="22"/>
       <c r="C62" s="21"/>
       <c r="D62" s="21"/>
-      <c r="E62" s="72">
-        <v>0</v>
-      </c>
-      <c r="F62" s="72">
-        <v>0</v>
-      </c>
-      <c r="G62" s="72">
-        <v>0</v>
-      </c>
-      <c r="H62" s="72">
-        <v>0</v>
-      </c>
-      <c r="I62" s="72">
-        <v>0</v>
-      </c>
+      <c r="E62" s="46"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="46"/>
+      <c r="H62" s="46"/>
+      <c r="I62" s="46"/>
       <c r="J62" s="41"/>
       <c r="K62" s="38" t="s">
         <v>20</v>
@@ -3194,21 +2674,11 @@
       <c r="B63" s="22"/>
       <c r="C63" s="21"/>
       <c r="D63" s="21"/>
-      <c r="E63" s="72">
-        <v>0</v>
-      </c>
-      <c r="F63" s="72">
-        <v>0</v>
-      </c>
-      <c r="G63" s="72">
-        <v>0</v>
-      </c>
-      <c r="H63" s="72">
-        <v>0</v>
-      </c>
-      <c r="I63" s="72">
-        <v>0</v>
-      </c>
+      <c r="E63" s="46"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="46"/>
+      <c r="H63" s="46"/>
+      <c r="I63" s="46"/>
       <c r="J63" s="41"/>
       <c r="K63" s="38" t="s">
         <v>20</v>
@@ -3225,21 +2695,11 @@
       <c r="B64" s="22"/>
       <c r="C64" s="21"/>
       <c r="D64" s="21"/>
-      <c r="E64" s="72">
-        <v>0</v>
-      </c>
-      <c r="F64" s="72">
-        <v>0</v>
-      </c>
-      <c r="G64" s="72">
-        <v>0</v>
-      </c>
-      <c r="H64" s="72">
-        <v>0</v>
-      </c>
-      <c r="I64" s="72">
-        <v>0</v>
-      </c>
+      <c r="E64" s="46"/>
+      <c r="F64" s="46"/>
+      <c r="G64" s="46"/>
+      <c r="H64" s="46"/>
+      <c r="I64" s="46"/>
       <c r="J64" s="41"/>
       <c r="K64" s="38" t="s">
         <v>20</v>
@@ -3256,21 +2716,11 @@
       <c r="B65" s="22"/>
       <c r="C65" s="21"/>
       <c r="D65" s="21"/>
-      <c r="E65" s="72">
-        <v>0</v>
-      </c>
-      <c r="F65" s="72">
-        <v>0</v>
-      </c>
-      <c r="G65" s="72">
-        <v>0</v>
-      </c>
-      <c r="H65" s="72">
-        <v>0</v>
-      </c>
-      <c r="I65" s="72">
-        <v>0</v>
-      </c>
+      <c r="E65" s="46"/>
+      <c r="F65" s="46"/>
+      <c r="G65" s="46"/>
+      <c r="H65" s="46"/>
+      <c r="I65" s="46"/>
       <c r="J65" s="41"/>
       <c r="K65" s="38" t="s">
         <v>20</v>
@@ -3287,21 +2737,11 @@
       <c r="B66" s="22"/>
       <c r="C66" s="21"/>
       <c r="D66" s="21"/>
-      <c r="E66" s="72">
-        <v>0</v>
-      </c>
-      <c r="F66" s="72">
-        <v>0</v>
-      </c>
-      <c r="G66" s="72">
-        <v>0</v>
-      </c>
-      <c r="H66" s="72">
-        <v>0</v>
-      </c>
-      <c r="I66" s="72">
-        <v>0</v>
-      </c>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="46"/>
+      <c r="I66" s="46"/>
       <c r="J66" s="41"/>
       <c r="K66" s="38" t="s">
         <v>20</v>
@@ -3318,21 +2758,11 @@
       <c r="B67" s="22"/>
       <c r="C67" s="21"/>
       <c r="D67" s="21"/>
-      <c r="E67" s="72">
-        <v>0</v>
-      </c>
-      <c r="F67" s="72">
-        <v>0</v>
-      </c>
-      <c r="G67" s="72">
-        <v>0</v>
-      </c>
-      <c r="H67" s="72">
-        <v>0</v>
-      </c>
-      <c r="I67" s="72">
-        <v>0</v>
-      </c>
+      <c r="E67" s="46"/>
+      <c r="F67" s="46"/>
+      <c r="G67" s="46"/>
+      <c r="H67" s="46"/>
+      <c r="I67" s="46"/>
       <c r="J67" s="41"/>
       <c r="K67" s="38" t="s">
         <v>20</v>
@@ -3349,21 +2779,11 @@
       <c r="B68" s="22"/>
       <c r="C68" s="21"/>
       <c r="D68" s="21"/>
-      <c r="E68" s="72">
-        <v>0</v>
-      </c>
-      <c r="F68" s="72">
-        <v>0</v>
-      </c>
-      <c r="G68" s="72">
-        <v>0</v>
-      </c>
-      <c r="H68" s="72">
-        <v>0</v>
-      </c>
-      <c r="I68" s="72">
-        <v>0</v>
-      </c>
+      <c r="E68" s="46"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="46"/>
+      <c r="H68" s="46"/>
+      <c r="I68" s="46"/>
       <c r="J68" s="41"/>
       <c r="K68" s="38" t="s">
         <v>20</v>
@@ -3380,21 +2800,11 @@
       <c r="B69" s="22"/>
       <c r="C69" s="21"/>
       <c r="D69" s="21"/>
-      <c r="E69" s="72">
-        <v>0</v>
-      </c>
-      <c r="F69" s="72">
-        <v>0</v>
-      </c>
-      <c r="G69" s="72">
-        <v>0</v>
-      </c>
-      <c r="H69" s="72">
-        <v>0</v>
-      </c>
-      <c r="I69" s="72">
-        <v>0</v>
-      </c>
+      <c r="E69" s="46"/>
+      <c r="F69" s="46"/>
+      <c r="G69" s="46"/>
+      <c r="H69" s="46"/>
+      <c r="I69" s="46"/>
       <c r="J69" s="41"/>
       <c r="K69" s="38" t="s">
         <v>20</v>
@@ -3411,21 +2821,11 @@
       <c r="B70" s="23"/>
       <c r="C70" s="24"/>
       <c r="D70" s="25"/>
-      <c r="E70" s="72">
-        <v>0</v>
-      </c>
-      <c r="F70" s="72">
-        <v>0</v>
-      </c>
-      <c r="G70" s="72">
-        <v>0</v>
-      </c>
-      <c r="H70" s="72">
-        <v>0</v>
-      </c>
-      <c r="I70" s="72">
-        <v>0</v>
-      </c>
+      <c r="E70" s="46"/>
+      <c r="F70" s="46"/>
+      <c r="G70" s="46"/>
+      <c r="H70" s="46"/>
+      <c r="I70" s="46"/>
       <c r="J70" s="43"/>
       <c r="K70" s="44" t="s">
         <v>20</v>
@@ -3436,11 +2836,11 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="46" t="s">
+      <c r="A71" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B71" s="46"/>
-      <c r="C71" s="46"/>
+      <c r="B71" s="54"/>
+      <c r="C71" s="54"/>
       <c r="D71" s="26"/>
       <c r="E71" s="27"/>
       <c r="F71" s="27"/>
@@ -3471,28 +2871,21 @@
       <c r="A74" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="47"/>
-      <c r="D74" s="47"/>
+      <c r="C74" s="55"/>
+      <c r="D74" s="55"/>
       <c r="E74" s="6"/>
       <c r="F74" s="6"/>
       <c r="G74" s="31"/>
       <c r="H74" s="6"/>
-      <c r="I74" s="48" t="s">
+      <c r="I74" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="J74" s="48"/>
-      <c r="K74" s="48"/>
-      <c r="L74" s="48"/>
+      <c r="J74" s="56"/>
+      <c r="K74" s="56"/>
+      <c r="L74" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="L5:M5"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="I74:L74"/>
@@ -3508,6 +2901,13 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="L5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" orientation="portrait" r:id="rId1"/>
@@ -3538,20 +2938,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
       <c r="M1" s="1"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3560,9 +2960,9 @@
       <c r="C2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
       <c r="G2" s="33"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
@@ -3572,20 +2972,20 @@
       <c r="M2" s="3"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="70" t="s">
+      <c r="A3" s="51" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="70"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
+      <c r="B3" s="51"/>
+      <c r="C3" s="51"/>
+      <c r="D3" s="51"/>
+      <c r="E3" s="51"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="51"/>
+      <c r="J3" s="51"/>
+      <c r="K3" s="51"/>
+      <c r="L3" s="51"/>
       <c r="M3" s="5"/>
     </row>
     <row r="4" spans="1:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3595,110 +2995,110 @@
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="71"/>
-      <c r="H5" s="71"/>
-      <c r="I5" s="71"/>
-      <c r="J5" s="71"/>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
       <c r="K5" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="52" t="s">
+      <c r="L5" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="52"/>
+      <c r="M5" s="53"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="51"/>
-      <c r="D6" s="51"/>
-      <c r="E6" s="51"/>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="51"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="47"/>
+      <c r="G6" s="47"/>
+      <c r="H6" s="47"/>
+      <c r="I6" s="47"/>
       <c r="J6" s="8"/>
       <c r="K6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="67"/>
-      <c r="M6" s="67"/>
+      <c r="L6" s="48"/>
+      <c r="M6" s="48"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="51"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="47"/>
+      <c r="G7" s="47"/>
+      <c r="H7" s="47"/>
+      <c r="I7" s="47"/>
       <c r="J7" s="9"/>
       <c r="K7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="52"/>
-      <c r="M7" s="52"/>
+      <c r="L7" s="53"/>
+      <c r="M7" s="53"/>
     </row>
     <row r="8" spans="1:13" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K8" s="34"/>
     </row>
     <row r="9" spans="1:13" s="11" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="53" t="s">
+      <c r="A9" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="55" t="s">
+      <c r="B9" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="57" t="s">
+      <c r="C9" s="63" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="59" t="s">
+      <c r="D9" s="65" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="61" t="s">
+      <c r="E9" s="67" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="49" t="s">
+      <c r="F9" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="50"/>
-      <c r="H9" s="63" t="s">
+      <c r="G9" s="58"/>
+      <c r="H9" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="63" t="s">
+      <c r="I9" s="69" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="65" t="s">
+      <c r="J9" s="71" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="66"/>
-      <c r="L9" s="65" t="s">
+      <c r="K9" s="72"/>
+      <c r="L9" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="66"/>
+      <c r="M9" s="72"/>
     </row>
     <row r="10" spans="1:13" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="54"/>
-      <c r="B10" s="56"/>
-      <c r="C10" s="58"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="62"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="62"/>
+      <c r="C10" s="64"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="68"/>
       <c r="F10" s="35" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="64"/>
-      <c r="I10" s="64"/>
+      <c r="H10" s="70"/>
+      <c r="I10" s="70"/>
       <c r="J10" s="12" t="s">
         <v>18</v>
       </c>
@@ -3719,21 +3119,11 @@
       <c r="B11" s="15"/>
       <c r="C11" s="16"/>
       <c r="D11" s="16"/>
-      <c r="E11" s="72">
-        <v>0</v>
-      </c>
-      <c r="F11" s="72">
-        <v>0</v>
-      </c>
-      <c r="G11" s="72">
-        <v>0</v>
-      </c>
-      <c r="H11" s="72">
-        <v>0</v>
-      </c>
-      <c r="I11" s="72">
-        <v>0</v>
-      </c>
+      <c r="E11" s="46"/>
+      <c r="F11" s="46"/>
+      <c r="G11" s="46"/>
+      <c r="H11" s="46"/>
+      <c r="I11" s="46"/>
       <c r="J11" s="37"/>
       <c r="K11" s="38" t="s">
         <v>20</v>
@@ -3750,21 +3140,11 @@
       <c r="B12" s="18"/>
       <c r="C12" s="19"/>
       <c r="D12" s="19"/>
-      <c r="E12" s="72">
-        <v>0</v>
-      </c>
-      <c r="F12" s="72">
-        <v>0</v>
-      </c>
-      <c r="G12" s="72">
-        <v>0</v>
-      </c>
-      <c r="H12" s="72">
-        <v>0</v>
-      </c>
-      <c r="I12" s="72">
-        <v>0</v>
-      </c>
+      <c r="E12" s="46"/>
+      <c r="F12" s="46"/>
+      <c r="G12" s="46"/>
+      <c r="H12" s="46"/>
+      <c r="I12" s="46"/>
       <c r="J12" s="39"/>
       <c r="K12" s="38" t="s">
         <v>20</v>
@@ -3781,21 +3161,11 @@
       <c r="B13" s="18"/>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
-      <c r="E13" s="72">
-        <v>0</v>
-      </c>
-      <c r="F13" s="72">
-        <v>0</v>
-      </c>
-      <c r="G13" s="72">
-        <v>0</v>
-      </c>
-      <c r="H13" s="72">
-        <v>0</v>
-      </c>
-      <c r="I13" s="72">
-        <v>0</v>
-      </c>
+      <c r="E13" s="46"/>
+      <c r="F13" s="46"/>
+      <c r="G13" s="46"/>
+      <c r="H13" s="46"/>
+      <c r="I13" s="46"/>
       <c r="J13" s="39"/>
       <c r="K13" s="38" t="s">
         <v>20</v>
@@ -3812,21 +3182,11 @@
       <c r="B14" s="18"/>
       <c r="C14" s="19"/>
       <c r="D14" s="19"/>
-      <c r="E14" s="72">
-        <v>0</v>
-      </c>
-      <c r="F14" s="72">
-        <v>0</v>
-      </c>
-      <c r="G14" s="72">
-        <v>0</v>
-      </c>
-      <c r="H14" s="72">
-        <v>0</v>
-      </c>
-      <c r="I14" s="72">
-        <v>0</v>
-      </c>
+      <c r="E14" s="46"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
       <c r="J14" s="39"/>
       <c r="K14" s="38" t="s">
         <v>20</v>
@@ -3843,21 +3203,11 @@
       <c r="B15" s="18"/>
       <c r="C15" s="19"/>
       <c r="D15" s="19"/>
-      <c r="E15" s="72">
-        <v>0</v>
-      </c>
-      <c r="F15" s="72">
-        <v>0</v>
-      </c>
-      <c r="G15" s="72">
-        <v>0</v>
-      </c>
-      <c r="H15" s="72">
-        <v>0</v>
-      </c>
-      <c r="I15" s="72">
-        <v>0</v>
-      </c>
+      <c r="E15" s="46"/>
+      <c r="F15" s="46"/>
+      <c r="G15" s="46"/>
+      <c r="H15" s="46"/>
+      <c r="I15" s="46"/>
       <c r="J15" s="39"/>
       <c r="K15" s="38" t="s">
         <v>20</v>
@@ -3874,21 +3224,11 @@
       <c r="B16" s="18"/>
       <c r="C16" s="19"/>
       <c r="D16" s="19"/>
-      <c r="E16" s="72">
-        <v>0</v>
-      </c>
-      <c r="F16" s="72">
-        <v>0</v>
-      </c>
-      <c r="G16" s="72">
-        <v>0</v>
-      </c>
-      <c r="H16" s="72">
-        <v>0</v>
-      </c>
-      <c r="I16" s="72">
-        <v>0</v>
-      </c>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
       <c r="J16" s="39"/>
       <c r="K16" s="38" t="s">
         <v>20</v>
@@ -3905,21 +3245,11 @@
       <c r="B17" s="18"/>
       <c r="C17" s="19"/>
       <c r="D17" s="19"/>
-      <c r="E17" s="72">
-        <v>0</v>
-      </c>
-      <c r="F17" s="72">
-        <v>0</v>
-      </c>
-      <c r="G17" s="72">
-        <v>0</v>
-      </c>
-      <c r="H17" s="72">
-        <v>0</v>
-      </c>
-      <c r="I17" s="72">
-        <v>0</v>
-      </c>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="46"/>
+      <c r="I17" s="46"/>
       <c r="J17" s="39"/>
       <c r="K17" s="38" t="s">
         <v>20</v>
@@ -3936,21 +3266,11 @@
       <c r="B18" s="18"/>
       <c r="C18" s="19"/>
       <c r="D18" s="19"/>
-      <c r="E18" s="72">
-        <v>0</v>
-      </c>
-      <c r="F18" s="72">
-        <v>0</v>
-      </c>
-      <c r="G18" s="72">
-        <v>0</v>
-      </c>
-      <c r="H18" s="72">
-        <v>0</v>
-      </c>
-      <c r="I18" s="72">
-        <v>0</v>
-      </c>
+      <c r="E18" s="46"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
       <c r="J18" s="39"/>
       <c r="K18" s="38" t="s">
         <v>20</v>
@@ -3967,21 +3287,11 @@
       <c r="B19" s="18"/>
       <c r="C19" s="19"/>
       <c r="D19" s="19"/>
-      <c r="E19" s="72">
-        <v>0</v>
-      </c>
-      <c r="F19" s="72">
-        <v>0</v>
-      </c>
-      <c r="G19" s="72">
-        <v>0</v>
-      </c>
-      <c r="H19" s="72">
-        <v>0</v>
-      </c>
-      <c r="I19" s="72">
-        <v>0</v>
-      </c>
+      <c r="E19" s="46"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="46"/>
       <c r="J19" s="39"/>
       <c r="K19" s="38" t="s">
         <v>20</v>
@@ -3998,21 +3308,11 @@
       <c r="B20" s="18"/>
       <c r="C20" s="19"/>
       <c r="D20" s="19"/>
-      <c r="E20" s="72">
-        <v>0</v>
-      </c>
-      <c r="F20" s="72">
-        <v>0</v>
-      </c>
-      <c r="G20" s="72">
-        <v>0</v>
-      </c>
-      <c r="H20" s="72">
-        <v>0</v>
-      </c>
-      <c r="I20" s="72">
-        <v>0</v>
-      </c>
+      <c r="E20" s="46"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
       <c r="J20" s="39"/>
       <c r="K20" s="38" t="s">
         <v>20</v>
@@ -4029,21 +3329,11 @@
       <c r="B21" s="18"/>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
-      <c r="E21" s="72">
-        <v>0</v>
-      </c>
-      <c r="F21" s="72">
-        <v>0</v>
-      </c>
-      <c r="G21" s="72">
-        <v>0</v>
-      </c>
-      <c r="H21" s="72">
-        <v>0</v>
-      </c>
-      <c r="I21" s="72">
-        <v>0</v>
-      </c>
+      <c r="E21" s="46"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
       <c r="J21" s="39"/>
       <c r="K21" s="38" t="s">
         <v>20</v>
@@ -4060,21 +3350,11 @@
       <c r="B22" s="18"/>
       <c r="C22" s="19"/>
       <c r="D22" s="19"/>
-      <c r="E22" s="72">
-        <v>0</v>
-      </c>
-      <c r="F22" s="72">
-        <v>0</v>
-      </c>
-      <c r="G22" s="72">
-        <v>0</v>
-      </c>
-      <c r="H22" s="72">
-        <v>0</v>
-      </c>
-      <c r="I22" s="72">
-        <v>0</v>
-      </c>
+      <c r="E22" s="46"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
       <c r="J22" s="39"/>
       <c r="K22" s="38" t="s">
         <v>20</v>
@@ -4091,21 +3371,11 @@
       <c r="B23" s="18"/>
       <c r="C23" s="19"/>
       <c r="D23" s="19"/>
-      <c r="E23" s="72">
-        <v>0</v>
-      </c>
-      <c r="F23" s="72">
-        <v>0</v>
-      </c>
-      <c r="G23" s="72">
-        <v>0</v>
-      </c>
-      <c r="H23" s="72">
-        <v>0</v>
-      </c>
-      <c r="I23" s="72">
-        <v>0</v>
-      </c>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
       <c r="J23" s="39"/>
       <c r="K23" s="38" t="s">
         <v>20</v>
@@ -4122,21 +3392,11 @@
       <c r="B24" s="20"/>
       <c r="C24" s="21"/>
       <c r="D24" s="21"/>
-      <c r="E24" s="72">
-        <v>0</v>
-      </c>
-      <c r="F24" s="72">
-        <v>0</v>
-      </c>
-      <c r="G24" s="72">
-        <v>0</v>
-      </c>
-      <c r="H24" s="72">
-        <v>0</v>
-      </c>
-      <c r="I24" s="72">
-        <v>0</v>
-      </c>
+      <c r="E24" s="46"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
       <c r="J24" s="40"/>
       <c r="K24" s="38" t="s">
         <v>20</v>
@@ -4153,21 +3413,11 @@
       <c r="B25" s="20"/>
       <c r="C25" s="21"/>
       <c r="D25" s="21"/>
-      <c r="E25" s="72">
-        <v>0</v>
-      </c>
-      <c r="F25" s="72">
-        <v>0</v>
-      </c>
-      <c r="G25" s="72">
-        <v>0</v>
-      </c>
-      <c r="H25" s="72">
-        <v>0</v>
-      </c>
-      <c r="I25" s="72">
-        <v>0</v>
-      </c>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
       <c r="J25" s="40"/>
       <c r="K25" s="38" t="s">
         <v>20</v>
@@ -4184,21 +3434,11 @@
       <c r="B26" s="20"/>
       <c r="C26" s="21"/>
       <c r="D26" s="21"/>
-      <c r="E26" s="72">
-        <v>0</v>
-      </c>
-      <c r="F26" s="72">
-        <v>0</v>
-      </c>
-      <c r="G26" s="72">
-        <v>0</v>
-      </c>
-      <c r="H26" s="72">
-        <v>0</v>
-      </c>
-      <c r="I26" s="72">
-        <v>0</v>
-      </c>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
       <c r="J26" s="41"/>
       <c r="K26" s="38" t="s">
         <v>20</v>
@@ -4215,21 +3455,11 @@
       <c r="B27" s="20"/>
       <c r="C27" s="21"/>
       <c r="D27" s="21"/>
-      <c r="E27" s="72">
-        <v>0</v>
-      </c>
-      <c r="F27" s="72">
-        <v>0</v>
-      </c>
-      <c r="G27" s="72">
-        <v>0</v>
-      </c>
-      <c r="H27" s="72">
-        <v>0</v>
-      </c>
-      <c r="I27" s="72">
-        <v>0</v>
-      </c>
+      <c r="E27" s="46"/>
+      <c r="F27" s="46"/>
+      <c r="G27" s="46"/>
+      <c r="H27" s="46"/>
+      <c r="I27" s="46"/>
       <c r="J27" s="40"/>
       <c r="K27" s="38" t="s">
         <v>20</v>
@@ -4246,21 +3476,11 @@
       <c r="B28" s="20"/>
       <c r="C28" s="21"/>
       <c r="D28" s="21"/>
-      <c r="E28" s="72">
-        <v>0</v>
-      </c>
-      <c r="F28" s="72">
-        <v>0</v>
-      </c>
-      <c r="G28" s="72">
-        <v>0</v>
-      </c>
-      <c r="H28" s="72">
-        <v>0</v>
-      </c>
-      <c r="I28" s="72">
-        <v>0</v>
-      </c>
+      <c r="E28" s="46"/>
+      <c r="F28" s="46"/>
+      <c r="G28" s="46"/>
+      <c r="H28" s="46"/>
+      <c r="I28" s="46"/>
       <c r="J28" s="41"/>
       <c r="K28" s="38" t="s">
         <v>20</v>
@@ -4277,21 +3497,11 @@
       <c r="B29" s="20"/>
       <c r="C29" s="21"/>
       <c r="D29" s="21"/>
-      <c r="E29" s="72">
-        <v>0</v>
-      </c>
-      <c r="F29" s="72">
-        <v>0</v>
-      </c>
-      <c r="G29" s="72">
-        <v>0</v>
-      </c>
-      <c r="H29" s="72">
-        <v>0</v>
-      </c>
-      <c r="I29" s="72">
-        <v>0</v>
-      </c>
+      <c r="E29" s="46"/>
+      <c r="F29" s="46"/>
+      <c r="G29" s="46"/>
+      <c r="H29" s="46"/>
+      <c r="I29" s="46"/>
       <c r="J29" s="41"/>
       <c r="K29" s="38" t="s">
         <v>20</v>
@@ -4308,21 +3518,11 @@
       <c r="B30" s="20"/>
       <c r="C30" s="21"/>
       <c r="D30" s="21"/>
-      <c r="E30" s="72">
-        <v>0</v>
-      </c>
-      <c r="F30" s="72">
-        <v>0</v>
-      </c>
-      <c r="G30" s="72">
-        <v>0</v>
-      </c>
-      <c r="H30" s="72">
-        <v>0</v>
-      </c>
-      <c r="I30" s="72">
-        <v>0</v>
-      </c>
+      <c r="E30" s="46"/>
+      <c r="F30" s="46"/>
+      <c r="G30" s="46"/>
+      <c r="H30" s="46"/>
+      <c r="I30" s="46"/>
       <c r="J30" s="41"/>
       <c r="K30" s="38" t="s">
         <v>20</v>
@@ -4339,21 +3539,11 @@
       <c r="B31" s="20"/>
       <c r="C31" s="21"/>
       <c r="D31" s="21"/>
-      <c r="E31" s="72">
-        <v>0</v>
-      </c>
-      <c r="F31" s="72">
-        <v>0</v>
-      </c>
-      <c r="G31" s="72">
-        <v>0</v>
-      </c>
-      <c r="H31" s="72">
-        <v>0</v>
-      </c>
-      <c r="I31" s="72">
-        <v>0</v>
-      </c>
+      <c r="E31" s="46"/>
+      <c r="F31" s="46"/>
+      <c r="G31" s="46"/>
+      <c r="H31" s="46"/>
+      <c r="I31" s="46"/>
       <c r="J31" s="41"/>
       <c r="K31" s="38" t="s">
         <v>20</v>
@@ -4370,21 +3560,11 @@
       <c r="B32" s="20"/>
       <c r="C32" s="21"/>
       <c r="D32" s="21"/>
-      <c r="E32" s="72">
-        <v>0</v>
-      </c>
-      <c r="F32" s="72">
-        <v>0</v>
-      </c>
-      <c r="G32" s="72">
-        <v>0</v>
-      </c>
-      <c r="H32" s="72">
-        <v>0</v>
-      </c>
-      <c r="I32" s="72">
-        <v>0</v>
-      </c>
+      <c r="E32" s="46"/>
+      <c r="F32" s="46"/>
+      <c r="G32" s="46"/>
+      <c r="H32" s="46"/>
+      <c r="I32" s="46"/>
       <c r="J32" s="40"/>
       <c r="K32" s="38" t="s">
         <v>20</v>
@@ -4401,21 +3581,11 @@
       <c r="B33" s="20"/>
       <c r="C33" s="21"/>
       <c r="D33" s="21"/>
-      <c r="E33" s="72">
-        <v>0</v>
-      </c>
-      <c r="F33" s="72">
-        <v>0</v>
-      </c>
-      <c r="G33" s="72">
-        <v>0</v>
-      </c>
-      <c r="H33" s="72">
-        <v>0</v>
-      </c>
-      <c r="I33" s="72">
-        <v>0</v>
-      </c>
+      <c r="E33" s="46"/>
+      <c r="F33" s="46"/>
+      <c r="G33" s="46"/>
+      <c r="H33" s="46"/>
+      <c r="I33" s="46"/>
       <c r="J33" s="40"/>
       <c r="K33" s="38" t="s">
         <v>20</v>
@@ -4432,21 +3602,11 @@
       <c r="B34" s="20"/>
       <c r="C34" s="21"/>
       <c r="D34" s="21"/>
-      <c r="E34" s="72">
-        <v>0</v>
-      </c>
-      <c r="F34" s="72">
-        <v>0</v>
-      </c>
-      <c r="G34" s="72">
-        <v>0</v>
-      </c>
-      <c r="H34" s="72">
-        <v>0</v>
-      </c>
-      <c r="I34" s="72">
-        <v>0</v>
-      </c>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="46"/>
+      <c r="I34" s="46"/>
       <c r="J34" s="41"/>
       <c r="K34" s="38" t="s">
         <v>20</v>
@@ -4463,21 +3623,11 @@
       <c r="B35" s="20"/>
       <c r="C35" s="21"/>
       <c r="D35" s="21"/>
-      <c r="E35" s="72">
-        <v>0</v>
-      </c>
-      <c r="F35" s="72">
-        <v>0</v>
-      </c>
-      <c r="G35" s="72">
-        <v>0</v>
-      </c>
-      <c r="H35" s="72">
-        <v>0</v>
-      </c>
-      <c r="I35" s="72">
-        <v>0</v>
-      </c>
+      <c r="E35" s="46"/>
+      <c r="F35" s="46"/>
+      <c r="G35" s="46"/>
+      <c r="H35" s="46"/>
+      <c r="I35" s="46"/>
       <c r="J35" s="40"/>
       <c r="K35" s="38" t="s">
         <v>20</v>
@@ -4494,21 +3644,11 @@
       <c r="B36" s="20"/>
       <c r="C36" s="21"/>
       <c r="D36" s="21"/>
-      <c r="E36" s="72">
-        <v>0</v>
-      </c>
-      <c r="F36" s="72">
-        <v>0</v>
-      </c>
-      <c r="G36" s="72">
-        <v>0</v>
-      </c>
-      <c r="H36" s="72">
-        <v>0</v>
-      </c>
-      <c r="I36" s="72">
-        <v>0</v>
-      </c>
+      <c r="E36" s="46"/>
+      <c r="F36" s="46"/>
+      <c r="G36" s="46"/>
+      <c r="H36" s="46"/>
+      <c r="I36" s="46"/>
       <c r="J36" s="41"/>
       <c r="K36" s="38" t="s">
         <v>20</v>
@@ -4525,21 +3665,11 @@
       <c r="B37" s="20"/>
       <c r="C37" s="21"/>
       <c r="D37" s="21"/>
-      <c r="E37" s="72">
-        <v>0</v>
-      </c>
-      <c r="F37" s="72">
-        <v>0</v>
-      </c>
-      <c r="G37" s="72">
-        <v>0</v>
-      </c>
-      <c r="H37" s="72">
-        <v>0</v>
-      </c>
-      <c r="I37" s="72">
-        <v>0</v>
-      </c>
+      <c r="E37" s="46"/>
+      <c r="F37" s="46"/>
+      <c r="G37" s="46"/>
+      <c r="H37" s="46"/>
+      <c r="I37" s="46"/>
       <c r="J37" s="41"/>
       <c r="K37" s="38" t="s">
         <v>20</v>
@@ -4556,21 +3686,11 @@
       <c r="B38" s="20"/>
       <c r="C38" s="21"/>
       <c r="D38" s="21"/>
-      <c r="E38" s="72">
-        <v>0</v>
-      </c>
-      <c r="F38" s="72">
-        <v>0</v>
-      </c>
-      <c r="G38" s="72">
-        <v>0</v>
-      </c>
-      <c r="H38" s="72">
-        <v>0</v>
-      </c>
-      <c r="I38" s="72">
-        <v>0</v>
-      </c>
+      <c r="E38" s="46"/>
+      <c r="F38" s="46"/>
+      <c r="G38" s="46"/>
+      <c r="H38" s="46"/>
+      <c r="I38" s="46"/>
       <c r="J38" s="41"/>
       <c r="K38" s="38" t="s">
         <v>20</v>
@@ -4587,21 +3707,11 @@
       <c r="B39" s="20"/>
       <c r="C39" s="21"/>
       <c r="D39" s="21"/>
-      <c r="E39" s="72">
-        <v>0</v>
-      </c>
-      <c r="F39" s="72">
-        <v>0</v>
-      </c>
-      <c r="G39" s="72">
-        <v>0</v>
-      </c>
-      <c r="H39" s="72">
-        <v>0</v>
-      </c>
-      <c r="I39" s="72">
-        <v>0</v>
-      </c>
+      <c r="E39" s="46"/>
+      <c r="F39" s="46"/>
+      <c r="G39" s="46"/>
+      <c r="H39" s="46"/>
+      <c r="I39" s="46"/>
       <c r="J39" s="40"/>
       <c r="K39" s="38" t="s">
         <v>20</v>
@@ -4618,21 +3728,11 @@
       <c r="B40" s="20"/>
       <c r="C40" s="21"/>
       <c r="D40" s="21"/>
-      <c r="E40" s="72">
-        <v>0</v>
-      </c>
-      <c r="F40" s="72">
-        <v>0</v>
-      </c>
-      <c r="G40" s="72">
-        <v>0</v>
-      </c>
-      <c r="H40" s="72">
-        <v>0</v>
-      </c>
-      <c r="I40" s="72">
-        <v>0</v>
-      </c>
+      <c r="E40" s="46"/>
+      <c r="F40" s="46"/>
+      <c r="G40" s="46"/>
+      <c r="H40" s="46"/>
+      <c r="I40" s="46"/>
       <c r="J40" s="40"/>
       <c r="K40" s="38" t="s">
         <v>20</v>
@@ -4649,21 +3749,11 @@
       <c r="B41" s="20"/>
       <c r="C41" s="21"/>
       <c r="D41" s="21"/>
-      <c r="E41" s="72">
-        <v>0</v>
-      </c>
-      <c r="F41" s="72">
-        <v>0</v>
-      </c>
-      <c r="G41" s="72">
-        <v>0</v>
-      </c>
-      <c r="H41" s="72">
-        <v>0</v>
-      </c>
-      <c r="I41" s="72">
-        <v>0</v>
-      </c>
+      <c r="E41" s="46"/>
+      <c r="F41" s="46"/>
+      <c r="G41" s="46"/>
+      <c r="H41" s="46"/>
+      <c r="I41" s="46"/>
       <c r="J41" s="40"/>
       <c r="K41" s="38" t="s">
         <v>20</v>
@@ -4680,21 +3770,11 @@
       <c r="B42" s="20"/>
       <c r="C42" s="21"/>
       <c r="D42" s="21"/>
-      <c r="E42" s="72">
-        <v>0</v>
-      </c>
-      <c r="F42" s="72">
-        <v>0</v>
-      </c>
-      <c r="G42" s="72">
-        <v>0</v>
-      </c>
-      <c r="H42" s="72">
-        <v>0</v>
-      </c>
-      <c r="I42" s="72">
-        <v>0</v>
-      </c>
+      <c r="E42" s="46"/>
+      <c r="F42" s="46"/>
+      <c r="G42" s="46"/>
+      <c r="H42" s="46"/>
+      <c r="I42" s="46"/>
       <c r="J42" s="41"/>
       <c r="K42" s="38" t="s">
         <v>20</v>
@@ -4711,21 +3791,11 @@
       <c r="B43" s="20"/>
       <c r="C43" s="21"/>
       <c r="D43" s="21"/>
-      <c r="E43" s="72">
-        <v>0</v>
-      </c>
-      <c r="F43" s="72">
-        <v>0</v>
-      </c>
-      <c r="G43" s="72">
-        <v>0</v>
-      </c>
-      <c r="H43" s="72">
-        <v>0</v>
-      </c>
-      <c r="I43" s="72">
-        <v>0</v>
-      </c>
+      <c r="E43" s="46"/>
+      <c r="F43" s="46"/>
+      <c r="G43" s="46"/>
+      <c r="H43" s="46"/>
+      <c r="I43" s="46"/>
       <c r="J43" s="40"/>
       <c r="K43" s="38" t="s">
         <v>20</v>
@@ -4742,21 +3812,11 @@
       <c r="B44" s="20"/>
       <c r="C44" s="21"/>
       <c r="D44" s="21"/>
-      <c r="E44" s="72">
-        <v>0</v>
-      </c>
-      <c r="F44" s="72">
-        <v>0</v>
-      </c>
-      <c r="G44" s="72">
-        <v>0</v>
-      </c>
-      <c r="H44" s="72">
-        <v>0</v>
-      </c>
-      <c r="I44" s="72">
-        <v>0</v>
-      </c>
+      <c r="E44" s="46"/>
+      <c r="F44" s="46"/>
+      <c r="G44" s="46"/>
+      <c r="H44" s="46"/>
+      <c r="I44" s="46"/>
       <c r="J44" s="41"/>
       <c r="K44" s="38" t="s">
         <v>20</v>
@@ -4773,21 +3833,11 @@
       <c r="B45" s="20"/>
       <c r="C45" s="21"/>
       <c r="D45" s="21"/>
-      <c r="E45" s="72">
-        <v>0</v>
-      </c>
-      <c r="F45" s="72">
-        <v>0</v>
-      </c>
-      <c r="G45" s="72">
-        <v>0</v>
-      </c>
-      <c r="H45" s="72">
-        <v>0</v>
-      </c>
-      <c r="I45" s="72">
-        <v>0</v>
-      </c>
+      <c r="E45" s="46"/>
+      <c r="F45" s="46"/>
+      <c r="G45" s="46"/>
+      <c r="H45" s="46"/>
+      <c r="I45" s="46"/>
       <c r="J45" s="40"/>
       <c r="K45" s="38" t="s">
         <v>20</v>
@@ -4804,21 +3854,11 @@
       <c r="B46" s="22"/>
       <c r="C46" s="21"/>
       <c r="D46" s="21"/>
-      <c r="E46" s="72">
-        <v>0</v>
-      </c>
-      <c r="F46" s="72">
-        <v>0</v>
-      </c>
-      <c r="G46" s="72">
-        <v>0</v>
-      </c>
-      <c r="H46" s="72">
-        <v>0</v>
-      </c>
-      <c r="I46" s="72">
-        <v>0</v>
-      </c>
+      <c r="E46" s="46"/>
+      <c r="F46" s="46"/>
+      <c r="G46" s="46"/>
+      <c r="H46" s="46"/>
+      <c r="I46" s="46"/>
       <c r="J46" s="41"/>
       <c r="K46" s="38" t="s">
         <v>20</v>
@@ -4835,21 +3875,11 @@
       <c r="B47" s="22"/>
       <c r="C47" s="21"/>
       <c r="D47" s="21"/>
-      <c r="E47" s="72">
-        <v>0</v>
-      </c>
-      <c r="F47" s="72">
-        <v>0</v>
-      </c>
-      <c r="G47" s="72">
-        <v>0</v>
-      </c>
-      <c r="H47" s="72">
-        <v>0</v>
-      </c>
-      <c r="I47" s="72">
-        <v>0</v>
-      </c>
+      <c r="E47" s="46"/>
+      <c r="F47" s="46"/>
+      <c r="G47" s="46"/>
+      <c r="H47" s="46"/>
+      <c r="I47" s="46"/>
       <c r="J47" s="41"/>
       <c r="K47" s="38" t="s">
         <v>20</v>
@@ -4866,21 +3896,11 @@
       <c r="B48" s="22"/>
       <c r="C48" s="21"/>
       <c r="D48" s="21"/>
-      <c r="E48" s="72">
-        <v>0</v>
-      </c>
-      <c r="F48" s="72">
-        <v>0</v>
-      </c>
-      <c r="G48" s="72">
-        <v>0</v>
-      </c>
-      <c r="H48" s="72">
-        <v>0</v>
-      </c>
-      <c r="I48" s="72">
-        <v>0</v>
-      </c>
+      <c r="E48" s="46"/>
+      <c r="F48" s="46"/>
+      <c r="G48" s="46"/>
+      <c r="H48" s="46"/>
+      <c r="I48" s="46"/>
       <c r="J48" s="41"/>
       <c r="K48" s="38" t="s">
         <v>20</v>
@@ -4897,21 +3917,11 @@
       <c r="B49" s="22"/>
       <c r="C49" s="21"/>
       <c r="D49" s="21"/>
-      <c r="E49" s="72">
-        <v>0</v>
-      </c>
-      <c r="F49" s="72">
-        <v>0</v>
-      </c>
-      <c r="G49" s="72">
-        <v>0</v>
-      </c>
-      <c r="H49" s="72">
-        <v>0</v>
-      </c>
-      <c r="I49" s="72">
-        <v>0</v>
-      </c>
+      <c r="E49" s="46"/>
+      <c r="F49" s="46"/>
+      <c r="G49" s="46"/>
+      <c r="H49" s="46"/>
+      <c r="I49" s="46"/>
       <c r="J49" s="41"/>
       <c r="K49" s="38" t="s">
         <v>20</v>
@@ -4928,21 +3938,11 @@
       <c r="B50" s="22"/>
       <c r="C50" s="21"/>
       <c r="D50" s="21"/>
-      <c r="E50" s="72">
-        <v>0</v>
-      </c>
-      <c r="F50" s="72">
-        <v>0</v>
-      </c>
-      <c r="G50" s="72">
-        <v>0</v>
-      </c>
-      <c r="H50" s="72">
-        <v>0</v>
-      </c>
-      <c r="I50" s="72">
-        <v>0</v>
-      </c>
+      <c r="E50" s="46"/>
+      <c r="F50" s="46"/>
+      <c r="G50" s="46"/>
+      <c r="H50" s="46"/>
+      <c r="I50" s="46"/>
       <c r="J50" s="41"/>
       <c r="K50" s="38" t="s">
         <v>20</v>
@@ -4959,21 +3959,11 @@
       <c r="B51" s="22"/>
       <c r="C51" s="21"/>
       <c r="D51" s="21"/>
-      <c r="E51" s="72">
-        <v>0</v>
-      </c>
-      <c r="F51" s="72">
-        <v>0</v>
-      </c>
-      <c r="G51" s="72">
-        <v>0</v>
-      </c>
-      <c r="H51" s="72">
-        <v>0</v>
-      </c>
-      <c r="I51" s="72">
-        <v>0</v>
-      </c>
+      <c r="E51" s="46"/>
+      <c r="F51" s="46"/>
+      <c r="G51" s="46"/>
+      <c r="H51" s="46"/>
+      <c r="I51" s="46"/>
       <c r="J51" s="41"/>
       <c r="K51" s="38" t="s">
         <v>20</v>
@@ -4990,21 +3980,11 @@
       <c r="B52" s="22"/>
       <c r="C52" s="21"/>
       <c r="D52" s="21"/>
-      <c r="E52" s="72">
-        <v>0</v>
-      </c>
-      <c r="F52" s="72">
-        <v>0</v>
-      </c>
-      <c r="G52" s="72">
-        <v>0</v>
-      </c>
-      <c r="H52" s="72">
-        <v>0</v>
-      </c>
-      <c r="I52" s="72">
-        <v>0</v>
-      </c>
+      <c r="E52" s="46"/>
+      <c r="F52" s="46"/>
+      <c r="G52" s="46"/>
+      <c r="H52" s="46"/>
+      <c r="I52" s="46"/>
       <c r="J52" s="41"/>
       <c r="K52" s="38" t="s">
         <v>20</v>
@@ -5021,21 +4001,11 @@
       <c r="B53" s="22"/>
       <c r="C53" s="21"/>
       <c r="D53" s="21"/>
-      <c r="E53" s="72">
-        <v>0</v>
-      </c>
-      <c r="F53" s="72">
-        <v>0</v>
-      </c>
-      <c r="G53" s="72">
-        <v>0</v>
-      </c>
-      <c r="H53" s="72">
-        <v>0</v>
-      </c>
-      <c r="I53" s="72">
-        <v>0</v>
-      </c>
+      <c r="E53" s="46"/>
+      <c r="F53" s="46"/>
+      <c r="G53" s="46"/>
+      <c r="H53" s="46"/>
+      <c r="I53" s="46"/>
       <c r="J53" s="41"/>
       <c r="K53" s="38" t="s">
         <v>20</v>
@@ -5052,21 +4022,11 @@
       <c r="B54" s="22"/>
       <c r="C54" s="21"/>
       <c r="D54" s="21"/>
-      <c r="E54" s="72">
-        <v>0</v>
-      </c>
-      <c r="F54" s="72">
-        <v>0</v>
-      </c>
-      <c r="G54" s="72">
-        <v>0</v>
-      </c>
-      <c r="H54" s="72">
-        <v>0</v>
-      </c>
-      <c r="I54" s="72">
-        <v>0</v>
-      </c>
+      <c r="E54" s="46"/>
+      <c r="F54" s="46"/>
+      <c r="G54" s="46"/>
+      <c r="H54" s="46"/>
+      <c r="I54" s="46"/>
       <c r="J54" s="41"/>
       <c r="K54" s="38" t="s">
         <v>20</v>
@@ -5083,21 +4043,11 @@
       <c r="B55" s="22"/>
       <c r="C55" s="21"/>
       <c r="D55" s="21"/>
-      <c r="E55" s="72">
-        <v>0</v>
-      </c>
-      <c r="F55" s="72">
-        <v>0</v>
-      </c>
-      <c r="G55" s="72">
-        <v>0</v>
-      </c>
-      <c r="H55" s="72">
-        <v>0</v>
-      </c>
-      <c r="I55" s="72">
-        <v>0</v>
-      </c>
+      <c r="E55" s="46"/>
+      <c r="F55" s="46"/>
+      <c r="G55" s="46"/>
+      <c r="H55" s="46"/>
+      <c r="I55" s="46"/>
       <c r="J55" s="41"/>
       <c r="K55" s="38" t="s">
         <v>20</v>
@@ -5114,21 +4064,11 @@
       <c r="B56" s="22"/>
       <c r="C56" s="21"/>
       <c r="D56" s="21"/>
-      <c r="E56" s="72">
-        <v>0</v>
-      </c>
-      <c r="F56" s="72">
-        <v>0</v>
-      </c>
-      <c r="G56" s="72">
-        <v>0</v>
-      </c>
-      <c r="H56" s="72">
-        <v>0</v>
-      </c>
-      <c r="I56" s="72">
-        <v>0</v>
-      </c>
+      <c r="E56" s="46"/>
+      <c r="F56" s="46"/>
+      <c r="G56" s="46"/>
+      <c r="H56" s="46"/>
+      <c r="I56" s="46"/>
       <c r="J56" s="41"/>
       <c r="K56" s="38" t="s">
         <v>20</v>
@@ -5145,21 +4085,11 @@
       <c r="B57" s="22"/>
       <c r="C57" s="21"/>
       <c r="D57" s="21"/>
-      <c r="E57" s="72">
-        <v>0</v>
-      </c>
-      <c r="F57" s="72">
-        <v>0</v>
-      </c>
-      <c r="G57" s="72">
-        <v>0</v>
-      </c>
-      <c r="H57" s="72">
-        <v>0</v>
-      </c>
-      <c r="I57" s="72">
-        <v>0</v>
-      </c>
+      <c r="E57" s="46"/>
+      <c r="F57" s="46"/>
+      <c r="G57" s="46"/>
+      <c r="H57" s="46"/>
+      <c r="I57" s="46"/>
       <c r="J57" s="41"/>
       <c r="K57" s="38" t="s">
         <v>20</v>
@@ -5176,21 +4106,11 @@
       <c r="B58" s="22"/>
       <c r="C58" s="21"/>
       <c r="D58" s="21"/>
-      <c r="E58" s="72">
-        <v>0</v>
-      </c>
-      <c r="F58" s="72">
-        <v>0</v>
-      </c>
-      <c r="G58" s="72">
-        <v>0</v>
-      </c>
-      <c r="H58" s="72">
-        <v>0</v>
-      </c>
-      <c r="I58" s="72">
-        <v>0</v>
-      </c>
+      <c r="E58" s="46"/>
+      <c r="F58" s="46"/>
+      <c r="G58" s="46"/>
+      <c r="H58" s="46"/>
+      <c r="I58" s="46"/>
       <c r="J58" s="41"/>
       <c r="K58" s="38" t="s">
         <v>20</v>
@@ -5207,21 +4127,11 @@
       <c r="B59" s="22"/>
       <c r="C59" s="21"/>
       <c r="D59" s="21"/>
-      <c r="E59" s="72">
-        <v>0</v>
-      </c>
-      <c r="F59" s="72">
-        <v>0</v>
-      </c>
-      <c r="G59" s="72">
-        <v>0</v>
-      </c>
-      <c r="H59" s="72">
-        <v>0</v>
-      </c>
-      <c r="I59" s="72">
-        <v>0</v>
-      </c>
+      <c r="E59" s="46"/>
+      <c r="F59" s="46"/>
+      <c r="G59" s="46"/>
+      <c r="H59" s="46"/>
+      <c r="I59" s="46"/>
       <c r="J59" s="41"/>
       <c r="K59" s="38" t="s">
         <v>20</v>
@@ -5238,21 +4148,11 @@
       <c r="B60" s="22"/>
       <c r="C60" s="21"/>
       <c r="D60" s="21"/>
-      <c r="E60" s="72">
-        <v>0</v>
-      </c>
-      <c r="F60" s="72">
-        <v>0</v>
-      </c>
-      <c r="G60" s="72">
-        <v>0</v>
-      </c>
-      <c r="H60" s="72">
-        <v>0</v>
-      </c>
-      <c r="I60" s="72">
-        <v>0</v>
-      </c>
+      <c r="E60" s="46"/>
+      <c r="F60" s="46"/>
+      <c r="G60" s="46"/>
+      <c r="H60" s="46"/>
+      <c r="I60" s="46"/>
       <c r="J60" s="41"/>
       <c r="K60" s="38" t="s">
         <v>20</v>
@@ -5269,21 +4169,11 @@
       <c r="B61" s="22"/>
       <c r="C61" s="21"/>
       <c r="D61" s="21"/>
-      <c r="E61" s="72">
-        <v>0</v>
-      </c>
-      <c r="F61" s="72">
-        <v>0</v>
-      </c>
-      <c r="G61" s="72">
-        <v>0</v>
-      </c>
-      <c r="H61" s="72">
-        <v>0</v>
-      </c>
-      <c r="I61" s="72">
-        <v>0</v>
-      </c>
+      <c r="E61" s="46"/>
+      <c r="F61" s="46"/>
+      <c r="G61" s="46"/>
+      <c r="H61" s="46"/>
+      <c r="I61" s="46"/>
       <c r="J61" s="41"/>
       <c r="K61" s="38" t="s">
         <v>20</v>
@@ -5300,21 +4190,11 @@
       <c r="B62" s="22"/>
       <c r="C62" s="21"/>
       <c r="D62" s="21"/>
-      <c r="E62" s="72">
-        <v>0</v>
-      </c>
-      <c r="F62" s="72">
-        <v>0</v>
-      </c>
-      <c r="G62" s="72">
-        <v>0</v>
-      </c>
-      <c r="H62" s="72">
-        <v>0</v>
-      </c>
-      <c r="I62" s="72">
-        <v>0</v>
-      </c>
+      <c r="E62" s="46"/>
+      <c r="F62" s="46"/>
+      <c r="G62" s="46"/>
+      <c r="H62" s="46"/>
+      <c r="I62" s="46"/>
       <c r="J62" s="41"/>
       <c r="K62" s="38" t="s">
         <v>20</v>
@@ -5331,21 +4211,11 @@
       <c r="B63" s="22"/>
       <c r="C63" s="21"/>
       <c r="D63" s="21"/>
-      <c r="E63" s="72">
-        <v>0</v>
-      </c>
-      <c r="F63" s="72">
-        <v>0</v>
-      </c>
-      <c r="G63" s="72">
-        <v>0</v>
-      </c>
-      <c r="H63" s="72">
-        <v>0</v>
-      </c>
-      <c r="I63" s="72">
-        <v>0</v>
-      </c>
+      <c r="E63" s="46"/>
+      <c r="F63" s="46"/>
+      <c r="G63" s="46"/>
+      <c r="H63" s="46"/>
+      <c r="I63" s="46"/>
       <c r="J63" s="41"/>
       <c r="K63" s="38" t="s">
         <v>20</v>
@@ -5362,21 +4232,11 @@
       <c r="B64" s="22"/>
       <c r="C64" s="21"/>
       <c r="D64" s="21"/>
-      <c r="E64" s="72">
-        <v>0</v>
-      </c>
-      <c r="F64" s="72">
-        <v>0</v>
-      </c>
-      <c r="G64" s="72">
-        <v>0</v>
-      </c>
-      <c r="H64" s="72">
-        <v>0</v>
-      </c>
-      <c r="I64" s="72">
-        <v>0</v>
-      </c>
+      <c r="E64" s="46"/>
+      <c r="F64" s="46"/>
+      <c r="G64" s="46"/>
+      <c r="H64" s="46"/>
+      <c r="I64" s="46"/>
       <c r="J64" s="41"/>
       <c r="K64" s="38" t="s">
         <v>20</v>
@@ -5393,21 +4253,11 @@
       <c r="B65" s="22"/>
       <c r="C65" s="21"/>
       <c r="D65" s="21"/>
-      <c r="E65" s="72">
-        <v>0</v>
-      </c>
-      <c r="F65" s="72">
-        <v>0</v>
-      </c>
-      <c r="G65" s="72">
-        <v>0</v>
-      </c>
-      <c r="H65" s="72">
-        <v>0</v>
-      </c>
-      <c r="I65" s="72">
-        <v>0</v>
-      </c>
+      <c r="E65" s="46"/>
+      <c r="F65" s="46"/>
+      <c r="G65" s="46"/>
+      <c r="H65" s="46"/>
+      <c r="I65" s="46"/>
       <c r="J65" s="41"/>
       <c r="K65" s="38" t="s">
         <v>20</v>
@@ -5424,21 +4274,11 @@
       <c r="B66" s="22"/>
       <c r="C66" s="21"/>
       <c r="D66" s="21"/>
-      <c r="E66" s="72">
-        <v>0</v>
-      </c>
-      <c r="F66" s="72">
-        <v>0</v>
-      </c>
-      <c r="G66" s="72">
-        <v>0</v>
-      </c>
-      <c r="H66" s="72">
-        <v>0</v>
-      </c>
-      <c r="I66" s="72">
-        <v>0</v>
-      </c>
+      <c r="E66" s="46"/>
+      <c r="F66" s="46"/>
+      <c r="G66" s="46"/>
+      <c r="H66" s="46"/>
+      <c r="I66" s="46"/>
       <c r="J66" s="41"/>
       <c r="K66" s="38" t="s">
         <v>20</v>
@@ -5455,21 +4295,11 @@
       <c r="B67" s="22"/>
       <c r="C67" s="21"/>
       <c r="D67" s="21"/>
-      <c r="E67" s="72">
-        <v>0</v>
-      </c>
-      <c r="F67" s="72">
-        <v>0</v>
-      </c>
-      <c r="G67" s="72">
-        <v>0</v>
-      </c>
-      <c r="H67" s="72">
-        <v>0</v>
-      </c>
-      <c r="I67" s="72">
-        <v>0</v>
-      </c>
+      <c r="E67" s="46"/>
+      <c r="F67" s="46"/>
+      <c r="G67" s="46"/>
+      <c r="H67" s="46"/>
+      <c r="I67" s="46"/>
       <c r="J67" s="41"/>
       <c r="K67" s="38" t="s">
         <v>20</v>
@@ -5486,21 +4316,11 @@
       <c r="B68" s="22"/>
       <c r="C68" s="21"/>
       <c r="D68" s="21"/>
-      <c r="E68" s="72">
-        <v>0</v>
-      </c>
-      <c r="F68" s="72">
-        <v>0</v>
-      </c>
-      <c r="G68" s="72">
-        <v>0</v>
-      </c>
-      <c r="H68" s="72">
-        <v>0</v>
-      </c>
-      <c r="I68" s="72">
-        <v>0</v>
-      </c>
+      <c r="E68" s="46"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="46"/>
+      <c r="H68" s="46"/>
+      <c r="I68" s="46"/>
       <c r="J68" s="41"/>
       <c r="K68" s="38" t="s">
         <v>20</v>
@@ -5517,21 +4337,11 @@
       <c r="B69" s="22"/>
       <c r="C69" s="21"/>
       <c r="D69" s="21"/>
-      <c r="E69" s="72">
-        <v>0</v>
-      </c>
-      <c r="F69" s="72">
-        <v>0</v>
-      </c>
-      <c r="G69" s="72">
-        <v>0</v>
-      </c>
-      <c r="H69" s="72">
-        <v>0</v>
-      </c>
-      <c r="I69" s="72">
-        <v>0</v>
-      </c>
+      <c r="E69" s="46"/>
+      <c r="F69" s="46"/>
+      <c r="G69" s="46"/>
+      <c r="H69" s="46"/>
+      <c r="I69" s="46"/>
       <c r="J69" s="41"/>
       <c r="K69" s="38" t="s">
         <v>20</v>
@@ -5548,21 +4358,11 @@
       <c r="B70" s="23"/>
       <c r="C70" s="24"/>
       <c r="D70" s="25"/>
-      <c r="E70" s="72">
-        <v>0</v>
-      </c>
-      <c r="F70" s="72">
-        <v>0</v>
-      </c>
-      <c r="G70" s="72">
-        <v>0</v>
-      </c>
-      <c r="H70" s="72">
-        <v>0</v>
-      </c>
-      <c r="I70" s="72">
-        <v>0</v>
-      </c>
+      <c r="E70" s="46"/>
+      <c r="F70" s="46"/>
+      <c r="G70" s="46"/>
+      <c r="H70" s="46"/>
+      <c r="I70" s="46"/>
       <c r="J70" s="43"/>
       <c r="K70" s="44" t="s">
         <v>20</v>
@@ -5573,11 +4373,11 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="46" t="s">
+      <c r="A71" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="B71" s="46"/>
-      <c r="C71" s="46"/>
+      <c r="B71" s="54"/>
+      <c r="C71" s="54"/>
       <c r="D71" s="26"/>
       <c r="E71" s="27"/>
       <c r="F71" s="27"/>
@@ -5608,26 +4408,28 @@
       <c r="A74" s="30" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="47"/>
-      <c r="D74" s="47"/>
+      <c r="C74" s="55"/>
+      <c r="D74" s="55"/>
       <c r="E74" s="34"/>
       <c r="F74" s="34"/>
       <c r="G74" s="34"/>
       <c r="H74" s="34"/>
-      <c r="I74" s="48" t="s">
+      <c r="I74" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="J74" s="48"/>
-      <c r="K74" s="48"/>
-      <c r="L74" s="48"/>
+      <c r="J74" s="56"/>
+      <c r="K74" s="56"/>
+      <c r="L74" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="L9:M9"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="C74:D74"/>
-    <mergeCell ref="I74:L74"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="L5:M5"/>
     <mergeCell ref="C7:I7"/>
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="A9:A10"/>
@@ -5638,13 +4440,11 @@
     <mergeCell ref="F9:G9"/>
     <mergeCell ref="H9:H10"/>
     <mergeCell ref="I9:I10"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="L9:M9"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="C74:D74"/>
+    <mergeCell ref="I74:L74"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Logos actualizados a imágenes
</commit_message>
<xml_diff>
--- a/public/formato_bac.xlsx
+++ b/public/formato_bac.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web\uc\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59000105-A821-4773-80F8-831DA4FDA579}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF47917-3563-43F5-8FB9-8D9EC3A48B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7F88D77E-4E3E-48C4-9DAA-2646452AF6C7}"/>
   </bookViews>
@@ -945,7 +945,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
+      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -953,13 +953,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="7915" t="27293" r="67234" b="33364"/>
+        <a:srcRect t="121" b="121"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="73269" y="21980"/>
-          <a:ext cx="1171395" cy="574433"/>
+          <a:ext cx="1180054" cy="576165"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -994,21 +994,21 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="76528" t="17588" r="7752" b="18173"/>
+        <a:srcRect l="51" r="51"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7850797" y="44707"/>
-          <a:ext cx="455737" cy="571450"/>
+          <a:off x="7855127" y="44707"/>
+          <a:ext cx="452273" cy="573182"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1048,7 +1048,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
+      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -1056,13 +1056,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="7915" t="27293" r="67234" b="33364"/>
+        <a:srcRect t="121" b="121"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="73269" y="21980"/>
-          <a:ext cx="1171395" cy="574433"/>
+          <a:ext cx="1180054" cy="576165"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1097,21 +1097,21 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="76528" t="17588" r="7752" b="18173"/>
+        <a:srcRect l="51" r="51"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7850797" y="44707"/>
-          <a:ext cx="455737" cy="571450"/>
+          <a:off x="7855127" y="44707"/>
+          <a:ext cx="452273" cy="573182"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1151,7 +1151,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
+      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -1159,13 +1159,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="7915" t="27293" r="67234" b="33364"/>
+        <a:srcRect t="121" b="121"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="73269" y="21980"/>
-          <a:ext cx="1171395" cy="574433"/>
+          <a:ext cx="1180054" cy="576165"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1200,21 +1200,21 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="76528" t="17588" r="7752" b="18173"/>
+        <a:srcRect l="51" r="51"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7850797" y="44707"/>
-          <a:ext cx="455737" cy="571450"/>
+          <a:off x="7855127" y="44707"/>
+          <a:ext cx="452273" cy="573182"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1254,7 +1254,7 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
+      <xdr:blipFill>
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
@@ -1262,13 +1262,13 @@
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="7915" t="27293" r="67234" b="33364"/>
+        <a:srcRect t="121" b="121"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
           <a:off x="73269" y="21980"/>
-          <a:ext cx="1171395" cy="574433"/>
+          <a:ext cx="1180054" cy="576165"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1303,21 +1303,21 @@
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
-      <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect l="76528" t="17588" r="7752" b="18173"/>
+        <a:srcRect l="51" r="51"/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7850797" y="44707"/>
-          <a:ext cx="455737" cy="571450"/>
+          <a:off x="7855127" y="44707"/>
+          <a:ext cx="452273" cy="573182"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1631,7 +1631,7 @@
   </sheetPr>
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:J5"/>
     </sheetView>
   </sheetViews>
@@ -3168,7 +3168,7 @@
   </sheetPr>
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:J5"/>
     </sheetView>
   </sheetViews>
@@ -4705,7 +4705,7 @@
   </sheetPr>
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:J5"/>
     </sheetView>
   </sheetViews>
@@ -6242,7 +6242,7 @@
   </sheetPr>
   <dimension ref="A1:M74"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C5" sqref="C5:J5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cambiado el logo otra vez
</commit_message>
<xml_diff>
--- a/public/formato_bac.xlsx
+++ b/public/formato_bac.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Web\uc\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBF47917-3563-43F5-8FB9-8D9EC3A48B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB2DC549-8417-4B2E-B3FE-5FB944C62305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7F88D77E-4E3E-48C4-9DAA-2646452AF6C7}"/>
   </bookViews>
@@ -600,7 +600,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="93">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -812,34 +812,55 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -881,24 +902,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -919,55 +922,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>73269</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>21980</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>292164</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>43963</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="14" name="Imagen 13">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1D7E0C4B-C76C-45A2-8175-65F109FFD03B}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:srcRect t="121" b="121"/>
-        <a:stretch/>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="73269" y="21980"/>
-          <a:ext cx="1180054" cy="576165"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
@@ -995,7 +949,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1017,30 +971,20 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>73269</xdr:colOff>
+      <xdr:colOff>43295</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>21980</xdr:rowOff>
+      <xdr:rowOff>44213</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>292164</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>43963</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="864892" cy="569664"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="9" name="Imagen 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74147713-7244-42FE-BBC4-C66DCE8FA96D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F5599E43-139B-4B7E-B6CB-BCF4B6B127EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1049,20 +993,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect t="121" b="121"/>
+        <a:srcRect/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="73269" y="21980"/>
-          <a:ext cx="1180054" cy="576165"/>
+          <a:off x="43295" y="44213"/>
+          <a:ext cx="864892" cy="569664"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1070,7 +1014,12 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
@@ -1098,7 +1047,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1120,30 +1069,20 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>73269</xdr:colOff>
+      <xdr:colOff>43295</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>21980</xdr:rowOff>
+      <xdr:rowOff>44213</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>292164</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>43963</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="864892" cy="569664"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="7" name="Imagen 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{621056C3-2329-4C04-9CE3-D8B61AF606E8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{836BC968-A74F-44D4-A0B6-7B082B56D432}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1152,20 +1091,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect t="121" b="121"/>
+        <a:srcRect/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="73269" y="21980"/>
-          <a:ext cx="1180054" cy="576165"/>
+          <a:off x="43295" y="44213"/>
+          <a:ext cx="864892" cy="569664"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1173,7 +1112,12 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
@@ -1189,10 +1133,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4">
+        <xdr:cNvPr id="6" name="Imagen 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{808B9AE4-5D1F-45F2-A728-8218BD3B6594}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FFCCE131-A391-4457-B4F9-0897FA828DFD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1201,7 +1145,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1223,30 +1167,20 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
+  <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>73269</xdr:colOff>
+      <xdr:colOff>43295</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>21980</xdr:rowOff>
+      <xdr:rowOff>44213</xdr:rowOff>
     </xdr:from>
-    <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>292164</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>43963</xdr:rowOff>
-    </xdr:to>
+    <xdr:ext cx="864891" cy="569664"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Imagen 3">
+        <xdr:cNvPr id="7" name="Imagen 13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC8E86A4-47C2-4962-9E2E-E00FAE916DCC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{440EDCD7-4807-4830-8A0F-4254DC675706}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1255,20 +1189,20 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
-        <a:srcRect t="121" b="121"/>
+        <a:srcRect/>
         <a:stretch/>
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="73269" y="21980"/>
-          <a:ext cx="1180054" cy="576165"/>
+          <a:off x="43295" y="44213"/>
+          <a:ext cx="864891" cy="569664"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1276,7 +1210,12 @@
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
-  </xdr:twoCellAnchor>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>11</xdr:col>
@@ -1292,10 +1231,10 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Imagen 4">
+        <xdr:cNvPr id="6" name="Imagen 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75E6A9A6-BA69-4DD2-BC09-5E2BEEBFC363}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09F7CE3A-3DD5-44CF-8A4E-7748D9EEEBBA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1304,7 +1243,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
@@ -1326,6 +1265,50 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>43295</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>44213</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="864891" cy="569664"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Imagen 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{58DE9F6F-5179-4D70-BE48-5396E18FA6E1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="43295" y="44213"/>
+          <a:ext cx="864891" cy="569664"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1647,20 +1630,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
       <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1669,10 +1652,10 @@
       <c r="C2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="64"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="66"/>
       <c r="H2" s="61"/>
       <c r="I2" s="61"/>
       <c r="J2" s="62"/>
@@ -1681,21 +1664,21 @@
       <c r="M2" s="62"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="65"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="64"/>
     </row>
     <row r="4" spans="1:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="K4" s="60"/>
@@ -1704,110 +1687,110 @@
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
       <c r="K5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="72" t="s">
+      <c r="L5" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="72"/>
+      <c r="M5" s="73"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
       <c r="J6" s="6"/>
       <c r="K6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
       <c r="J7" s="7"/>
       <c r="K7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
     </row>
     <row r="8" spans="1:13" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:13" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="77" t="s">
+      <c r="C9" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="79" t="s">
+      <c r="D9" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="81" t="s">
+      <c r="E9" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="69" t="s">
+      <c r="F9" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="70"/>
-      <c r="H9" s="83" t="s">
+      <c r="G9" s="78"/>
+      <c r="H9" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="83" t="s">
+      <c r="I9" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="85" t="s">
+      <c r="J9" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="86"/>
-      <c r="L9" s="85" t="s">
+      <c r="K9" s="92"/>
+      <c r="L9" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="86"/>
+      <c r="M9" s="92"/>
     </row>
     <row r="10" spans="1:13" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="74"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="82"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="88"/>
       <c r="F10" s="25" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
       <c r="J10" s="10" t="s">
         <v>18</v>
       </c>
@@ -3082,11 +3065,11 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="66" t="s">
+      <c r="A71" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="B71" s="66"/>
-      <c r="C71" s="66"/>
+      <c r="B71" s="74"/>
+      <c r="C71" s="74"/>
       <c r="D71" s="18"/>
       <c r="E71" s="19"/>
       <c r="F71" s="19"/>
@@ -3117,28 +3100,21 @@
       <c r="A74" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="67"/>
-      <c r="D74" s="67"/>
+      <c r="C74" s="75"/>
+      <c r="D74" s="75"/>
       <c r="E74" s="4"/>
       <c r="F74" s="4"/>
       <c r="G74" s="23"/>
       <c r="H74" s="4"/>
-      <c r="I74" s="68" t="s">
+      <c r="I74" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="J74" s="68"/>
-      <c r="K74" s="68"/>
-      <c r="L74" s="68"/>
+      <c r="J74" s="76"/>
+      <c r="K74" s="76"/>
+      <c r="L74" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="L5:M5"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="I74:L74"/>
@@ -3154,6 +3130,13 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="L5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" orientation="portrait" r:id="rId1"/>
@@ -3184,20 +3167,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
       <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3206,10 +3189,10 @@
       <c r="C2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="64"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="66"/>
       <c r="H2" s="61"/>
       <c r="I2" s="61"/>
       <c r="J2" s="62"/>
@@ -3218,133 +3201,133 @@
       <c r="M2" s="62"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="65"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="64"/>
     </row>
     <row r="4" spans="1:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K4" s="24"/>
+      <c r="K4" s="65"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
       <c r="K5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="72" t="s">
+      <c r="L5" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="72"/>
+      <c r="M5" s="73"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
       <c r="J6" s="6"/>
       <c r="K6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
       <c r="J7" s="7"/>
       <c r="K7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
     </row>
     <row r="8" spans="1:13" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K8" s="24"/>
     </row>
     <row r="9" spans="1:13" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="77" t="s">
+      <c r="C9" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="79" t="s">
+      <c r="D9" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="81" t="s">
+      <c r="E9" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="69" t="s">
+      <c r="F9" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="70"/>
-      <c r="H9" s="83" t="s">
+      <c r="G9" s="78"/>
+      <c r="H9" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="83" t="s">
+      <c r="I9" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="85" t="s">
+      <c r="J9" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="86"/>
-      <c r="L9" s="85" t="s">
+      <c r="K9" s="92"/>
+      <c r="L9" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="86"/>
+      <c r="M9" s="92"/>
     </row>
     <row r="10" spans="1:13" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="74"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="82"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="88"/>
       <c r="F10" s="25" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
       <c r="J10" s="10" t="s">
         <v>18</v>
       </c>
@@ -4619,11 +4602,11 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="66" t="s">
+      <c r="A71" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="B71" s="66"/>
-      <c r="C71" s="66"/>
+      <c r="B71" s="74"/>
+      <c r="C71" s="74"/>
       <c r="D71" s="18"/>
       <c r="E71" s="19"/>
       <c r="F71" s="19"/>
@@ -4654,21 +4637,28 @@
       <c r="A74" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="67"/>
-      <c r="D74" s="67"/>
+      <c r="C74" s="75"/>
+      <c r="D74" s="75"/>
       <c r="E74" s="24"/>
       <c r="F74" s="24"/>
       <c r="G74" s="24"/>
       <c r="H74" s="24"/>
-      <c r="I74" s="68" t="s">
+      <c r="I74" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="J74" s="68"/>
-      <c r="K74" s="68"/>
-      <c r="L74" s="68"/>
+      <c r="J74" s="76"/>
+      <c r="K74" s="76"/>
+      <c r="L74" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="L5:M5"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="I74:L74"/>
@@ -4684,13 +4674,6 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="L5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" orientation="portrait" r:id="rId1"/>
@@ -4721,20 +4704,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
       <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -4743,10 +4726,10 @@
       <c r="C2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="64"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="66"/>
       <c r="H2" s="61"/>
       <c r="I2" s="61"/>
       <c r="J2" s="62"/>
@@ -4755,133 +4738,133 @@
       <c r="M2" s="62"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="65"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="64"/>
     </row>
     <row r="4" spans="1:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K4" s="37"/>
+      <c r="K4" s="65"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
       <c r="K5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="72" t="s">
+      <c r="L5" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="72"/>
+      <c r="M5" s="73"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
       <c r="J6" s="6"/>
       <c r="K6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
       <c r="J7" s="7"/>
       <c r="K7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
     </row>
     <row r="8" spans="1:13" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K8" s="37"/>
     </row>
     <row r="9" spans="1:13" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="77" t="s">
+      <c r="C9" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="79" t="s">
+      <c r="D9" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="81" t="s">
+      <c r="E9" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="69" t="s">
+      <c r="F9" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="70"/>
-      <c r="H9" s="83" t="s">
+      <c r="G9" s="78"/>
+      <c r="H9" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="83" t="s">
+      <c r="I9" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="85" t="s">
+      <c r="J9" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="86"/>
-      <c r="L9" s="85" t="s">
+      <c r="K9" s="92"/>
+      <c r="L9" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="86"/>
+      <c r="M9" s="92"/>
     </row>
     <row r="10" spans="1:13" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="74"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="82"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="88"/>
       <c r="F10" s="25" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
       <c r="J10" s="10" t="s">
         <v>18</v>
       </c>
@@ -6156,11 +6139,11 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="66" t="s">
+      <c r="A71" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="B71" s="66"/>
-      <c r="C71" s="66"/>
+      <c r="B71" s="74"/>
+      <c r="C71" s="74"/>
       <c r="D71" s="18"/>
       <c r="E71" s="19"/>
       <c r="F71" s="19"/>
@@ -6191,21 +6174,28 @@
       <c r="A74" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="67"/>
-      <c r="D74" s="67"/>
+      <c r="C74" s="75"/>
+      <c r="D74" s="75"/>
       <c r="E74" s="37"/>
       <c r="F74" s="37"/>
       <c r="G74" s="37"/>
       <c r="H74" s="37"/>
-      <c r="I74" s="68" t="s">
+      <c r="I74" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="J74" s="68"/>
-      <c r="K74" s="68"/>
-      <c r="L74" s="68"/>
+      <c r="J74" s="76"/>
+      <c r="K74" s="76"/>
+      <c r="L74" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="L5:M5"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="I74:L74"/>
@@ -6221,13 +6211,6 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="L5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" orientation="portrait" r:id="rId1"/>
@@ -6258,20 +6241,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="88"/>
-      <c r="C1" s="88"/>
-      <c r="D1" s="88"/>
-      <c r="E1" s="88"/>
-      <c r="F1" s="88"/>
-      <c r="G1" s="88"/>
-      <c r="H1" s="88"/>
-      <c r="I1" s="88"/>
-      <c r="J1" s="88"/>
-      <c r="K1" s="88"/>
-      <c r="L1" s="88"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
       <c r="M1" s="61"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -6280,10 +6263,10 @@
       <c r="C2" s="63" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="89"/>
-      <c r="E2" s="89"/>
-      <c r="F2" s="89"/>
-      <c r="G2" s="64"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="66"/>
       <c r="H2" s="61"/>
       <c r="I2" s="61"/>
       <c r="J2" s="62"/>
@@ -6292,133 +6275,133 @@
       <c r="M2" s="62"/>
     </row>
     <row r="3" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="90" t="s">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="90"/>
-      <c r="D3" s="90"/>
-      <c r="E3" s="90"/>
-      <c r="F3" s="90"/>
-      <c r="G3" s="90"/>
-      <c r="H3" s="90"/>
-      <c r="I3" s="90"/>
-      <c r="J3" s="90"/>
-      <c r="K3" s="90"/>
-      <c r="L3" s="90"/>
-      <c r="M3" s="65"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="64"/>
     </row>
     <row r="4" spans="1:13" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="K4" s="38"/>
+      <c r="K4" s="65"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="91"/>
-      <c r="D5" s="91"/>
-      <c r="E5" s="91"/>
-      <c r="F5" s="91"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="91"/>
-      <c r="I5" s="91"/>
-      <c r="J5" s="91"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
       <c r="K5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="72" t="s">
+      <c r="L5" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="M5" s="72"/>
+      <c r="M5" s="73"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="71"/>
-      <c r="H6" s="71"/>
-      <c r="I6" s="71"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
       <c r="J6" s="6"/>
       <c r="K6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="87"/>
-      <c r="M6" s="87"/>
+      <c r="L6" s="68"/>
+      <c r="M6" s="68"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="71"/>
-      <c r="H7" s="71"/>
-      <c r="I7" s="71"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="67"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="67"/>
+      <c r="H7" s="67"/>
+      <c r="I7" s="67"/>
       <c r="J7" s="7"/>
       <c r="K7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L7" s="72"/>
-      <c r="M7" s="72"/>
+      <c r="L7" s="73"/>
+      <c r="M7" s="73"/>
     </row>
     <row r="8" spans="1:13" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="K8" s="38"/>
     </row>
     <row r="9" spans="1:13" s="9" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="73" t="s">
+      <c r="A9" s="79" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="75" t="s">
+      <c r="B9" s="81" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="77" t="s">
+      <c r="C9" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="79" t="s">
+      <c r="D9" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="81" t="s">
+      <c r="E9" s="87" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="69" t="s">
+      <c r="F9" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="G9" s="70"/>
-      <c r="H9" s="83" t="s">
+      <c r="G9" s="78"/>
+      <c r="H9" s="89" t="s">
         <v>14</v>
       </c>
-      <c r="I9" s="83" t="s">
+      <c r="I9" s="89" t="s">
         <v>15</v>
       </c>
-      <c r="J9" s="85" t="s">
+      <c r="J9" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="K9" s="86"/>
-      <c r="L9" s="85" t="s">
+      <c r="K9" s="92"/>
+      <c r="L9" s="91" t="s">
         <v>17</v>
       </c>
-      <c r="M9" s="86"/>
+      <c r="M9" s="92"/>
     </row>
     <row r="10" spans="1:13" ht="11.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="74"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="78"/>
-      <c r="D10" s="80"/>
-      <c r="E10" s="82"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="82"/>
+      <c r="C10" s="84"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="88"/>
       <c r="F10" s="25" t="s">
         <v>28</v>
       </c>
       <c r="G10" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
+      <c r="H10" s="90"/>
+      <c r="I10" s="90"/>
       <c r="J10" s="10" t="s">
         <v>18</v>
       </c>
@@ -7693,11 +7676,11 @@
       </c>
     </row>
     <row r="71" spans="1:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="66" t="s">
+      <c r="A71" s="74" t="s">
         <v>21</v>
       </c>
-      <c r="B71" s="66"/>
-      <c r="C71" s="66"/>
+      <c r="B71" s="74"/>
+      <c r="C71" s="74"/>
       <c r="D71" s="18"/>
       <c r="E71" s="19"/>
       <c r="F71" s="19"/>
@@ -7728,21 +7711,28 @@
       <c r="A74" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="C74" s="67"/>
-      <c r="D74" s="67"/>
+      <c r="C74" s="75"/>
+      <c r="D74" s="75"/>
       <c r="E74" s="38"/>
       <c r="F74" s="38"/>
       <c r="G74" s="38"/>
       <c r="H74" s="38"/>
-      <c r="I74" s="68" t="s">
+      <c r="I74" s="76" t="s">
         <v>24</v>
       </c>
-      <c r="J74" s="68"/>
-      <c r="K74" s="68"/>
-      <c r="L74" s="68"/>
+      <c r="J74" s="76"/>
+      <c r="K74" s="76"/>
+      <c r="L74" s="76"/>
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C6:I6"/>
+    <mergeCell ref="L6:M6"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="A3:L3"/>
+    <mergeCell ref="C5:J5"/>
+    <mergeCell ref="L5:M5"/>
     <mergeCell ref="A71:C71"/>
     <mergeCell ref="C74:D74"/>
     <mergeCell ref="I74:L74"/>
@@ -7758,13 +7748,6 @@
     <mergeCell ref="I9:I10"/>
     <mergeCell ref="J9:K9"/>
     <mergeCell ref="L9:M9"/>
-    <mergeCell ref="C6:I6"/>
-    <mergeCell ref="L6:M6"/>
-    <mergeCell ref="A1:L1"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="A3:L3"/>
-    <mergeCell ref="C5:J5"/>
-    <mergeCell ref="L5:M5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="70" orientation="portrait" r:id="rId1"/>

</xml_diff>